<commit_message>
Register : continue coding functionnality
</commit_message>
<xml_diff>
--- a/uwwtd website/sites/all/modules/uwwtd/model/2015_register_model_20151102_2.xlsx
+++ b/uwwtd website/sites/all/modules/uwwtd/model/2015_register_model_20151102_2.xlsx
@@ -2381,7 +2381,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="62">
+  <borders count="68">
     <border>
       <left/>
       <right/>
@@ -3148,6 +3148,96 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3170,7 +3260,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="628">
+  <cellXfs count="633">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4237,9 +4327,6 @@
     <xf numFmtId="0" fontId="11" fillId="22" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -4279,17 +4366,6 @@
     <xf numFmtId="0" fontId="14" fillId="17" borderId="9" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="36" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
@@ -4428,48 +4504,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="6" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="7" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="7" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
@@ -4504,6 +4538,12 @@
     <xf numFmtId="3" fontId="11" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="4" fontId="17" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4549,17 +4589,119 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="6" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="7" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="7" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="33" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="33" fillId="13" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="33" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="33" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="33" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="33" fillId="13" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="33" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="33" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="33" fillId="23" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="33" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="30" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="12" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="20" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4573,107 +4715,41 @@
     <xf numFmtId="0" fontId="11" fillId="18" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="13" fillId="12" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="13" fillId="20" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="51" fillId="30" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="30" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="33" fillId="23" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="33" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="30" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="12" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="33" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="33" fillId="13" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="33" fillId="13" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="33" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="51" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="30" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="30" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="30" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="65" fillId="32" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4709,16 +4785,7 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="35" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="18" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4773,6 +4840,40 @@
     <xf numFmtId="3" fontId="13" fillId="12" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="59" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="59" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="62" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="63" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="63" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="65" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="66" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="66" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Hyperlink 2" xfId="10"/>
@@ -5270,186 +5371,186 @@
       <c r="AR3" s="5"/>
     </row>
     <row r="4" spans="1:44" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="507" t="s">
+      <c r="A4" s="501" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="508"/>
-      <c r="C4" s="508"/>
-      <c r="D4" s="508"/>
-      <c r="E4" s="509"/>
-      <c r="F4" s="509"/>
-      <c r="G4" s="509"/>
-      <c r="H4" s="509"/>
-      <c r="I4" s="509"/>
-      <c r="J4" s="509"/>
-      <c r="K4" s="509"/>
-      <c r="L4" s="509"/>
-      <c r="M4" s="509"/>
-      <c r="N4" s="509"/>
-      <c r="O4" s="509"/>
-      <c r="P4" s="509"/>
-      <c r="Q4" s="509"/>
-      <c r="R4" s="509"/>
-      <c r="S4" s="509"/>
-      <c r="T4" s="509"/>
-      <c r="U4" s="509"/>
-      <c r="V4" s="509"/>
-      <c r="W4" s="509"/>
-      <c r="X4" s="509"/>
-      <c r="Y4" s="509"/>
-      <c r="Z4" s="509"/>
-      <c r="AA4" s="509"/>
-      <c r="AB4" s="509"/>
-      <c r="AC4" s="509"/>
-      <c r="AD4" s="509"/>
-      <c r="AE4" s="509"/>
-      <c r="AF4" s="509"/>
-      <c r="AG4" s="509"/>
-      <c r="AH4" s="509"/>
-      <c r="AI4" s="509"/>
-      <c r="AJ4" s="509"/>
-      <c r="AK4" s="509"/>
-      <c r="AL4" s="509"/>
-      <c r="AM4" s="509"/>
-      <c r="AN4" s="509"/>
-      <c r="AO4" s="509"/>
-      <c r="AP4" s="509"/>
-      <c r="AQ4" s="510" t="s">
+      <c r="B4" s="502"/>
+      <c r="C4" s="502"/>
+      <c r="D4" s="502"/>
+      <c r="E4" s="503"/>
+      <c r="F4" s="503"/>
+      <c r="G4" s="503"/>
+      <c r="H4" s="503"/>
+      <c r="I4" s="503"/>
+      <c r="J4" s="503"/>
+      <c r="K4" s="503"/>
+      <c r="L4" s="503"/>
+      <c r="M4" s="503"/>
+      <c r="N4" s="503"/>
+      <c r="O4" s="503"/>
+      <c r="P4" s="503"/>
+      <c r="Q4" s="503"/>
+      <c r="R4" s="503"/>
+      <c r="S4" s="503"/>
+      <c r="T4" s="503"/>
+      <c r="U4" s="503"/>
+      <c r="V4" s="503"/>
+      <c r="W4" s="503"/>
+      <c r="X4" s="503"/>
+      <c r="Y4" s="503"/>
+      <c r="Z4" s="503"/>
+      <c r="AA4" s="503"/>
+      <c r="AB4" s="503"/>
+      <c r="AC4" s="503"/>
+      <c r="AD4" s="503"/>
+      <c r="AE4" s="503"/>
+      <c r="AF4" s="503"/>
+      <c r="AG4" s="503"/>
+      <c r="AH4" s="503"/>
+      <c r="AI4" s="503"/>
+      <c r="AJ4" s="503"/>
+      <c r="AK4" s="503"/>
+      <c r="AL4" s="503"/>
+      <c r="AM4" s="503"/>
+      <c r="AN4" s="503"/>
+      <c r="AO4" s="503"/>
+      <c r="AP4" s="503"/>
+      <c r="AQ4" s="504" t="s">
         <v>3</v>
       </c>
-      <c r="AR4" s="510"/>
+      <c r="AR4" s="504"/>
     </row>
     <row r="5" spans="1:44" ht="135" x14ac:dyDescent="0.25">
-      <c r="A5" s="504" t="s">
+      <c r="A5" s="498" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="504" t="s">
+      <c r="B5" s="498" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="504" t="s">
+      <c r="C5" s="498" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="505" t="s">
+      <c r="D5" s="499" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="504" t="s">
+      <c r="E5" s="498" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="504" t="s">
+      <c r="F5" s="498" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="504" t="s">
+      <c r="G5" s="498" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="504" t="s">
+      <c r="H5" s="498" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="504" t="s">
+      <c r="I5" s="498" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="504" t="s">
+      <c r="J5" s="498" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="504" t="s">
+      <c r="K5" s="498" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="504" t="s">
+      <c r="L5" s="498" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="504" t="s">
+      <c r="M5" s="498" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="504" t="s">
+      <c r="N5" s="498" t="s">
         <v>17</v>
       </c>
-      <c r="O5" s="504" t="s">
+      <c r="O5" s="498" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="504" t="s">
+      <c r="P5" s="498" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="504" t="s">
+      <c r="Q5" s="498" t="s">
         <v>20</v>
       </c>
-      <c r="R5" s="504" t="s">
+      <c r="R5" s="498" t="s">
         <v>21</v>
       </c>
-      <c r="S5" s="504" t="s">
+      <c r="S5" s="498" t="s">
         <v>22</v>
       </c>
-      <c r="T5" s="504" t="s">
+      <c r="T5" s="498" t="s">
         <v>23</v>
       </c>
-      <c r="U5" s="504" t="s">
+      <c r="U5" s="498" t="s">
         <v>24</v>
       </c>
-      <c r="V5" s="504" t="s">
+      <c r="V5" s="498" t="s">
         <v>22</v>
       </c>
-      <c r="W5" s="504" t="s">
+      <c r="W5" s="498" t="s">
         <v>23</v>
       </c>
-      <c r="X5" s="504" t="s">
+      <c r="X5" s="498" t="s">
         <v>25</v>
       </c>
-      <c r="Y5" s="504" t="s">
+      <c r="Y5" s="498" t="s">
         <v>26</v>
       </c>
-      <c r="Z5" s="504" t="s">
+      <c r="Z5" s="498" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="504" t="s">
+      <c r="AA5" s="498" t="s">
         <v>28</v>
       </c>
-      <c r="AB5" s="504" t="s">
+      <c r="AB5" s="498" t="s">
         <v>29</v>
       </c>
-      <c r="AC5" s="504" t="s">
+      <c r="AC5" s="498" t="s">
         <v>30</v>
       </c>
-      <c r="AD5" s="504" t="s">
+      <c r="AD5" s="498" t="s">
         <v>31</v>
       </c>
-      <c r="AE5" s="504" t="s">
+      <c r="AE5" s="498" t="s">
         <v>32</v>
       </c>
-      <c r="AF5" s="504" t="s">
+      <c r="AF5" s="498" t="s">
         <v>33</v>
       </c>
-      <c r="AG5" s="504" t="s">
+      <c r="AG5" s="498" t="s">
         <v>34</v>
       </c>
-      <c r="AH5" s="504" t="s">
+      <c r="AH5" s="498" t="s">
         <v>35</v>
       </c>
-      <c r="AI5" s="504" t="s">
+      <c r="AI5" s="498" t="s">
         <v>36</v>
       </c>
-      <c r="AJ5" s="504" t="s">
+      <c r="AJ5" s="498" t="s">
         <v>37</v>
       </c>
-      <c r="AK5" s="504" t="s">
+      <c r="AK5" s="498" t="s">
         <v>38</v>
       </c>
-      <c r="AL5" s="504" t="s">
+      <c r="AL5" s="498" t="s">
         <v>39</v>
       </c>
-      <c r="AM5" s="504" t="s">
+      <c r="AM5" s="498" t="s">
         <v>40</v>
       </c>
-      <c r="AN5" s="505" t="s">
+      <c r="AN5" s="499" t="s">
         <v>41</v>
       </c>
-      <c r="AO5" s="505" t="s">
+      <c r="AO5" s="499" t="s">
         <v>42</v>
       </c>
-      <c r="AP5" s="505" t="s">
+      <c r="AP5" s="499" t="s">
         <v>43</v>
       </c>
-      <c r="AQ5" s="506" t="s">
+      <c r="AQ5" s="500" t="s">
         <v>44</v>
       </c>
-      <c r="AR5" s="506" t="s">
+      <c r="AR5" s="500" t="s">
         <v>45</v>
       </c>
     </row>
@@ -5491,103 +5592,103 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="465" t="s">
+      <c r="A3" s="459" t="s">
         <v>346</v>
       </c>
-      <c r="B3" s="466" t="s">
+      <c r="B3" s="460" t="s">
         <v>347</v>
       </c>
-      <c r="C3" s="467" t="s">
+      <c r="C3" s="461" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="468" t="s">
+      <c r="A4" s="462" t="s">
         <v>349</v>
       </c>
-      <c r="B4" s="469" t="s">
+      <c r="B4" s="463" t="s">
         <v>350</v>
       </c>
-      <c r="C4" s="470"/>
+      <c r="C4" s="464"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="471" t="s">
+      <c r="A5" s="465" t="s">
         <v>351</v>
       </c>
-      <c r="B5" s="472" t="s">
+      <c r="B5" s="466" t="s">
         <v>350</v>
       </c>
-      <c r="C5" s="473"/>
+      <c r="C5" s="467"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="471" t="s">
+      <c r="A6" s="465" t="s">
         <v>352</v>
       </c>
-      <c r="B6" s="472" t="s">
+      <c r="B6" s="466" t="s">
         <v>350</v>
       </c>
-      <c r="C6" s="473"/>
+      <c r="C6" s="467"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="471" t="s">
+      <c r="A7" s="465" t="s">
         <v>353</v>
       </c>
-      <c r="B7" s="472" t="s">
+      <c r="B7" s="466" t="s">
         <v>350</v>
       </c>
-      <c r="C7" s="473"/>
+      <c r="C7" s="467"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="471" t="s">
+      <c r="A8" s="465" t="s">
         <v>354</v>
       </c>
-      <c r="B8" s="472" t="s">
+      <c r="B8" s="466" t="s">
         <v>350</v>
       </c>
-      <c r="C8" s="474"/>
+      <c r="C8" s="468"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="471" t="s">
+      <c r="A9" s="465" t="s">
         <v>355</v>
       </c>
-      <c r="B9" s="472" t="s">
+      <c r="B9" s="466" t="s">
         <v>350</v>
       </c>
-      <c r="C9" s="474"/>
+      <c r="C9" s="468"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="471" t="s">
+      <c r="A10" s="465" t="s">
         <v>356</v>
       </c>
-      <c r="B10" s="472" t="s">
+      <c r="B10" s="466" t="s">
         <v>350</v>
       </c>
-      <c r="C10" s="474"/>
+      <c r="C10" s="468"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="471" t="s">
+      <c r="A11" s="465" t="s">
         <v>357</v>
       </c>
-      <c r="B11" s="472" t="s">
+      <c r="B11" s="466" t="s">
         <v>350</v>
       </c>
-      <c r="C11" s="475"/>
+      <c r="C11" s="469"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="471" t="s">
+      <c r="A12" s="465" t="s">
         <v>358</v>
       </c>
-      <c r="B12" s="472" t="s">
+      <c r="B12" s="466" t="s">
         <v>350</v>
       </c>
-      <c r="C12" s="475"/>
+      <c r="C12" s="469"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="476" t="s">
+      <c r="A13" s="470" t="s">
         <v>359</v>
       </c>
-      <c r="B13" s="477"/>
-      <c r="C13" s="478"/>
+      <c r="B13" s="471"/>
+      <c r="C13" s="472"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -5595,67 +5696,67 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A20" s="479" t="s">
+      <c r="A20" s="473" t="s">
         <v>346</v>
       </c>
-      <c r="B20" s="480" t="s">
+      <c r="B20" s="474" t="s">
         <v>347</v>
       </c>
-      <c r="C20" s="481" t="s">
+      <c r="C20" s="475" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="482" t="s">
+      <c r="A21" s="476" t="s">
         <v>110</v>
       </c>
-      <c r="B21" s="483" t="s">
+      <c r="B21" s="477" t="s">
         <v>361</v>
       </c>
-      <c r="C21" s="483"/>
+      <c r="C21" s="477"/>
     </row>
     <row r="22" spans="1:3" ht="39" x14ac:dyDescent="0.25">
-      <c r="A22" s="482" t="s">
+      <c r="A22" s="476" t="s">
         <v>362</v>
       </c>
-      <c r="B22" s="483" t="s">
+      <c r="B22" s="477" t="s">
         <v>363</v>
       </c>
-      <c r="C22" s="483"/>
+      <c r="C22" s="477"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="471" t="s">
+      <c r="A23" s="465" t="s">
         <v>364</v>
       </c>
-      <c r="B23" s="484" t="s">
+      <c r="B23" s="478" t="s">
         <v>365</v>
       </c>
-      <c r="C23" s="485"/>
+      <c r="C23" s="479"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="471" t="s">
+      <c r="A24" s="465" t="s">
         <v>366</v>
       </c>
-      <c r="B24" s="484" t="s">
+      <c r="B24" s="478" t="s">
         <v>365</v>
       </c>
-      <c r="C24" s="485"/>
+      <c r="C24" s="479"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="471" t="s">
+      <c r="A25" s="465" t="s">
         <v>367</v>
       </c>
-      <c r="B25" s="484" t="s">
+      <c r="B25" s="478" t="s">
         <v>365</v>
       </c>
-      <c r="C25" s="485"/>
+      <c r="C25" s="479"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="476" t="s">
+      <c r="A26" s="470" t="s">
         <v>359</v>
       </c>
-      <c r="B26" s="486"/>
-      <c r="C26" s="487"/>
+      <c r="B26" s="480"/>
+      <c r="C26" s="481"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5691,34 +5792,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="488" t="s">
+      <c r="A2" s="482" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="489"/>
-      <c r="C4" s="490"/>
-      <c r="D4" s="491"/>
+      <c r="B4" s="483"/>
+      <c r="C4" s="484"/>
+      <c r="D4" s="485"/>
     </row>
     <row r="5" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="492" t="s">
+      <c r="A5" s="486" t="s">
         <v>369</v>
       </c>
-      <c r="B5" s="492" t="s">
+      <c r="B5" s="486" t="s">
         <v>370</v>
       </c>
-      <c r="C5" s="492" t="s">
+      <c r="C5" s="486" t="s">
         <v>371</v>
       </c>
-      <c r="D5" s="492" t="s">
+      <c r="D5" s="486" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="493"/>
-      <c r="B6" s="494"/>
-      <c r="C6" s="495"/>
-      <c r="D6" s="496"/>
+      <c r="A6" s="487"/>
+      <c r="B6" s="488"/>
+      <c r="C6" s="489"/>
+      <c r="D6" s="490"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6">
@@ -5754,27 +5855,27 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="497"/>
+      <c r="A3" s="491"/>
     </row>
     <row r="5" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="492" t="s">
+      <c r="A5" s="486" t="s">
         <v>369</v>
       </c>
-      <c r="B5" s="492" t="s">
+      <c r="B5" s="486" t="s">
         <v>370</v>
       </c>
-      <c r="C5" s="492" t="s">
+      <c r="C5" s="486" t="s">
         <v>374</v>
       </c>
-      <c r="D5" s="492" t="s">
+      <c r="D5" s="486" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="498"/>
-      <c r="B6" s="499"/>
-      <c r="C6" s="500"/>
-      <c r="D6" s="501"/>
+      <c r="A6" s="492"/>
+      <c r="B6" s="493"/>
+      <c r="C6" s="494"/>
+      <c r="D6" s="495"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6:B6">
@@ -5803,37 +5904,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="488" t="s">
+      <c r="A2" s="482" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="492" t="s">
+      <c r="A4" s="486" t="s">
         <v>376</v>
       </c>
-      <c r="B4" s="492" t="s">
+      <c r="B4" s="486" t="s">
         <v>377</v>
       </c>
-      <c r="C4" s="492" t="s">
+      <c r="C4" s="486" t="s">
         <v>378</v>
       </c>
-      <c r="D4" s="492" t="s">
+      <c r="D4" s="486" t="s">
         <v>379</v>
       </c>
-      <c r="E4" s="492" t="s">
+      <c r="E4" s="486" t="s">
         <v>380</v>
       </c>
-      <c r="F4" s="492" t="s">
+      <c r="F4" s="486" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="498"/>
-      <c r="B5" s="502"/>
-      <c r="C5" s="502"/>
-      <c r="D5" s="502"/>
-      <c r="E5" s="503"/>
-      <c r="F5" s="501"/>
+      <c r="A5" s="492"/>
+      <c r="B5" s="496"/>
+      <c r="C5" s="496"/>
+      <c r="D5" s="496"/>
+      <c r="E5" s="497"/>
+      <c r="F5" s="495"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:D5">
@@ -5867,38 +5968,38 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="497"/>
+      <c r="A3" s="491"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="488"/>
+      <c r="A4" s="482"/>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="492" t="s">
+      <c r="A5" s="486" t="s">
         <v>376</v>
       </c>
-      <c r="B5" s="492" t="s">
+      <c r="B5" s="486" t="s">
         <v>377</v>
       </c>
-      <c r="C5" s="492" t="s">
+      <c r="C5" s="486" t="s">
         <v>378</v>
       </c>
-      <c r="D5" s="492" t="s">
+      <c r="D5" s="486" t="s">
         <v>379</v>
       </c>
-      <c r="E5" s="492" t="s">
+      <c r="E5" s="486" t="s">
         <v>380</v>
       </c>
-      <c r="F5" s="492" t="s">
+      <c r="F5" s="486" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="498"/>
-      <c r="B6" s="499"/>
-      <c r="C6" s="499"/>
-      <c r="D6" s="499"/>
-      <c r="E6" s="500"/>
-      <c r="F6" s="501"/>
+      <c r="A6" s="492"/>
+      <c r="B6" s="493"/>
+      <c r="C6" s="493"/>
+      <c r="D6" s="493"/>
+      <c r="E6" s="494"/>
+      <c r="F6" s="495"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6:D6">
@@ -5923,24 +6024,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:101" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="511" t="s">
+      <c r="A1" s="534" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="512"/>
-      <c r="C1" s="512"/>
-      <c r="D1" s="512"/>
-      <c r="E1" s="512"/>
-      <c r="F1" s="512"/>
-      <c r="G1" s="512"/>
-      <c r="H1" s="513" t="s">
+      <c r="B1" s="535"/>
+      <c r="C1" s="535"/>
+      <c r="D1" s="535"/>
+      <c r="E1" s="535"/>
+      <c r="F1" s="535"/>
+      <c r="G1" s="535"/>
+      <c r="H1" s="536" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="514"/>
-      <c r="J1" s="514"/>
-      <c r="K1" s="514"/>
-      <c r="L1" s="514"/>
-      <c r="M1" s="515"/>
-      <c r="N1" s="516" t="s">
+      <c r="I1" s="537"/>
+      <c r="J1" s="537"/>
+      <c r="K1" s="537"/>
+      <c r="L1" s="537"/>
+      <c r="M1" s="538"/>
+      <c r="N1" s="539" t="s">
         <v>50</v>
       </c>
       <c r="O1" s="517"/>
@@ -5949,31 +6050,31 @@
       <c r="R1" s="517"/>
       <c r="S1" s="517"/>
       <c r="T1" s="518"/>
-      <c r="U1" s="519" t="s">
+      <c r="U1" s="540" t="s">
         <v>51</v>
       </c>
-      <c r="V1" s="520"/>
-      <c r="W1" s="521"/>
-      <c r="X1" s="521"/>
-      <c r="Y1" s="522"/>
-      <c r="Z1" s="523" t="s">
+      <c r="V1" s="541"/>
+      <c r="W1" s="542"/>
+      <c r="X1" s="542"/>
+      <c r="Y1" s="543"/>
+      <c r="Z1" s="544" t="s">
         <v>52</v>
       </c>
-      <c r="AA1" s="524"/>
-      <c r="AB1" s="524"/>
-      <c r="AC1" s="524"/>
-      <c r="AD1" s="524"/>
-      <c r="AE1" s="524"/>
-      <c r="AF1" s="524"/>
-      <c r="AG1" s="524"/>
-      <c r="AH1" s="524"/>
-      <c r="AI1" s="524"/>
-      <c r="AJ1" s="524"/>
-      <c r="AK1" s="524"/>
-      <c r="AL1" s="524"/>
+      <c r="AA1" s="545"/>
+      <c r="AB1" s="545"/>
+      <c r="AC1" s="545"/>
+      <c r="AD1" s="545"/>
+      <c r="AE1" s="545"/>
+      <c r="AF1" s="545"/>
+      <c r="AG1" s="545"/>
+      <c r="AH1" s="545"/>
+      <c r="AI1" s="545"/>
+      <c r="AJ1" s="545"/>
+      <c r="AK1" s="545"/>
+      <c r="AL1" s="545"/>
       <c r="AM1" s="7"/>
       <c r="AN1" s="8"/>
-      <c r="AO1" s="536" t="s">
+      <c r="AO1" s="516" t="s">
         <v>53</v>
       </c>
       <c r="AP1" s="517"/>
@@ -5992,62 +6093,62 @@
       <c r="BA1" s="12"/>
       <c r="BB1" s="12"/>
       <c r="BC1" s="12"/>
-      <c r="BD1" s="543" t="s">
+      <c r="BD1" s="525" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="544"/>
-      <c r="BF1" s="544"/>
-      <c r="BG1" s="544"/>
-      <c r="BH1" s="544"/>
-      <c r="BI1" s="545"/>
-      <c r="BJ1" s="546" t="s">
+      <c r="BE1" s="526"/>
+      <c r="BF1" s="526"/>
+      <c r="BG1" s="526"/>
+      <c r="BH1" s="526"/>
+      <c r="BI1" s="527"/>
+      <c r="BJ1" s="528" t="s">
         <v>56</v>
       </c>
-      <c r="BK1" s="547"/>
-      <c r="BL1" s="547"/>
-      <c r="BM1" s="547"/>
-      <c r="BN1" s="547"/>
-      <c r="BO1" s="548"/>
-      <c r="BP1" s="549" t="s">
+      <c r="BK1" s="529"/>
+      <c r="BL1" s="529"/>
+      <c r="BM1" s="529"/>
+      <c r="BN1" s="529"/>
+      <c r="BO1" s="530"/>
+      <c r="BP1" s="531" t="s">
         <v>57</v>
       </c>
-      <c r="BQ1" s="550"/>
-      <c r="BR1" s="550"/>
-      <c r="BS1" s="550"/>
-      <c r="BT1" s="550"/>
-      <c r="BU1" s="550"/>
-      <c r="BV1" s="551"/>
-      <c r="BW1" s="525" t="s">
+      <c r="BQ1" s="532"/>
+      <c r="BR1" s="532"/>
+      <c r="BS1" s="532"/>
+      <c r="BT1" s="532"/>
+      <c r="BU1" s="532"/>
+      <c r="BV1" s="533"/>
+      <c r="BW1" s="505" t="s">
         <v>58</v>
       </c>
-      <c r="BX1" s="526"/>
-      <c r="BY1" s="526"/>
-      <c r="BZ1" s="526"/>
-      <c r="CA1" s="526"/>
-      <c r="CB1" s="526"/>
+      <c r="BX1" s="506"/>
+      <c r="BY1" s="506"/>
+      <c r="BZ1" s="506"/>
+      <c r="CA1" s="506"/>
+      <c r="CB1" s="506"/>
       <c r="CC1" s="8"/>
       <c r="CD1" s="13"/>
-      <c r="CE1" s="527" t="s">
+      <c r="CE1" s="507" t="s">
         <v>59</v>
       </c>
-      <c r="CF1" s="528"/>
-      <c r="CG1" s="528"/>
-      <c r="CH1" s="528"/>
-      <c r="CI1" s="528"/>
-      <c r="CJ1" s="528"/>
-      <c r="CK1" s="528"/>
-      <c r="CL1" s="529"/>
-      <c r="CM1" s="529"/>
-      <c r="CN1" s="529"/>
-      <c r="CO1" s="529"/>
-      <c r="CP1" s="529"/>
-      <c r="CQ1" s="529"/>
-      <c r="CR1" s="529"/>
-      <c r="CS1" s="529"/>
-      <c r="CT1" s="529"/>
-      <c r="CU1" s="529"/>
-      <c r="CV1" s="529"/>
-      <c r="CW1" s="529"/>
+      <c r="CF1" s="508"/>
+      <c r="CG1" s="508"/>
+      <c r="CH1" s="508"/>
+      <c r="CI1" s="508"/>
+      <c r="CJ1" s="508"/>
+      <c r="CK1" s="508"/>
+      <c r="CL1" s="509"/>
+      <c r="CM1" s="509"/>
+      <c r="CN1" s="509"/>
+      <c r="CO1" s="509"/>
+      <c r="CP1" s="509"/>
+      <c r="CQ1" s="509"/>
+      <c r="CR1" s="509"/>
+      <c r="CS1" s="509"/>
+      <c r="CT1" s="509"/>
+      <c r="CU1" s="509"/>
+      <c r="CV1" s="509"/>
+      <c r="CW1" s="509"/>
     </row>
     <row r="2" spans="1:101" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -6071,18 +6172,18 @@
       <c r="G2" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="530" t="s">
+      <c r="H2" s="510" t="s">
         <v>67</v>
       </c>
-      <c r="I2" s="531"/>
-      <c r="J2" s="531" t="s">
+      <c r="I2" s="511"/>
+      <c r="J2" s="511" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="531"/>
-      <c r="L2" s="531" t="s">
+      <c r="K2" s="511"/>
+      <c r="L2" s="511" t="s">
         <v>69</v>
       </c>
-      <c r="M2" s="532"/>
+      <c r="M2" s="512"/>
       <c r="N2" s="16" t="s">
         <v>60</v>
       </c>
@@ -6209,36 +6310,36 @@
       <c r="BC2" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="BD2" s="533" t="s">
+      <c r="BD2" s="513" t="s">
         <v>101</v>
       </c>
-      <c r="BE2" s="534"/>
-      <c r="BF2" s="534"/>
-      <c r="BG2" s="534" t="s">
+      <c r="BE2" s="514"/>
+      <c r="BF2" s="514"/>
+      <c r="BG2" s="514" t="s">
         <v>102</v>
       </c>
-      <c r="BH2" s="534"/>
-      <c r="BI2" s="535"/>
-      <c r="BJ2" s="537" t="s">
+      <c r="BH2" s="514"/>
+      <c r="BI2" s="515"/>
+      <c r="BJ2" s="519" t="s">
         <v>101</v>
       </c>
-      <c r="BK2" s="538"/>
-      <c r="BL2" s="538"/>
-      <c r="BM2" s="538" t="s">
+      <c r="BK2" s="520"/>
+      <c r="BL2" s="520"/>
+      <c r="BM2" s="520" t="s">
         <v>102</v>
       </c>
-      <c r="BN2" s="538"/>
-      <c r="BO2" s="539"/>
-      <c r="BP2" s="540" t="s">
+      <c r="BN2" s="520"/>
+      <c r="BO2" s="521"/>
+      <c r="BP2" s="522" t="s">
         <v>101</v>
       </c>
-      <c r="BQ2" s="541"/>
-      <c r="BR2" s="541"/>
-      <c r="BS2" s="541" t="s">
+      <c r="BQ2" s="523"/>
+      <c r="BR2" s="523"/>
+      <c r="BS2" s="523" t="s">
         <v>102</v>
       </c>
-      <c r="BT2" s="542"/>
-      <c r="BU2" s="542"/>
+      <c r="BT2" s="524"/>
+      <c r="BU2" s="524"/>
       <c r="BV2" s="31" t="s">
         <v>103</v>
       </c>
@@ -7165,6 +7266,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:T1"/>
+    <mergeCell ref="U1:Y1"/>
+    <mergeCell ref="Z1:AL1"/>
     <mergeCell ref="BW1:CB1"/>
     <mergeCell ref="CE1:CW1"/>
     <mergeCell ref="H2:I2"/>
@@ -7180,11 +7286,6 @@
     <mergeCell ref="BD1:BI1"/>
     <mergeCell ref="BJ1:BO1"/>
     <mergeCell ref="BP1:BV1"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:T1"/>
-    <mergeCell ref="U1:Y1"/>
-    <mergeCell ref="Z1:AL1"/>
   </mergeCells>
   <conditionalFormatting sqref="A13:A14 A4:B4">
     <cfRule type="duplicateValues" dxfId="8" priority="1"/>
@@ -7223,115 +7324,115 @@
         <v>150</v>
       </c>
       <c r="L1" s="111"/>
-      <c r="M1" s="556" t="s">
+      <c r="M1" s="572" t="s">
         <v>151</v>
       </c>
-      <c r="N1" s="557" t="s">
+      <c r="N1" s="573" t="s">
         <v>152</v>
       </c>
-      <c r="O1" s="558"/>
-      <c r="P1" s="558"/>
-      <c r="Q1" s="558"/>
-      <c r="R1" s="559" t="s">
+      <c r="O1" s="574"/>
+      <c r="P1" s="574"/>
+      <c r="Q1" s="574"/>
+      <c r="R1" s="575" t="s">
         <v>153</v>
       </c>
-      <c r="S1" s="560"/>
-      <c r="T1" s="560"/>
-      <c r="U1" s="560"/>
-      <c r="V1" s="560"/>
-      <c r="W1" s="560"/>
-      <c r="X1" s="561"/>
-      <c r="Y1" s="562" t="s">
+      <c r="S1" s="567"/>
+      <c r="T1" s="567"/>
+      <c r="U1" s="567"/>
+      <c r="V1" s="567"/>
+      <c r="W1" s="567"/>
+      <c r="X1" s="576"/>
+      <c r="Y1" s="556" t="s">
         <v>154</v>
       </c>
-      <c r="Z1" s="547"/>
-      <c r="AA1" s="565" t="s">
+      <c r="Z1" s="529"/>
+      <c r="AA1" s="577" t="s">
         <v>155</v>
       </c>
-      <c r="AB1" s="567" t="s">
+      <c r="AB1" s="568" t="s">
         <v>156</v>
       </c>
-      <c r="AC1" s="575" t="s">
+      <c r="AC1" s="563" t="s">
         <v>157</v>
       </c>
-      <c r="AD1" s="576"/>
-      <c r="AE1" s="576"/>
-      <c r="AF1" s="577"/>
-      <c r="AG1" s="578" t="s">
+      <c r="AD1" s="564"/>
+      <c r="AE1" s="564"/>
+      <c r="AF1" s="565"/>
+      <c r="AG1" s="566" t="s">
         <v>158</v>
       </c>
-      <c r="AH1" s="560"/>
-      <c r="AI1" s="560"/>
-      <c r="AJ1" s="560"/>
-      <c r="AK1" s="560"/>
-      <c r="AL1" s="560"/>
-      <c r="AM1" s="560"/>
-      <c r="AN1" s="560"/>
-      <c r="AO1" s="567" t="s">
+      <c r="AH1" s="567"/>
+      <c r="AI1" s="567"/>
+      <c r="AJ1" s="567"/>
+      <c r="AK1" s="567"/>
+      <c r="AL1" s="567"/>
+      <c r="AM1" s="567"/>
+      <c r="AN1" s="567"/>
+      <c r="AO1" s="568" t="s">
         <v>159</v>
       </c>
-      <c r="AP1" s="562" t="s">
+      <c r="AP1" s="556" t="s">
         <v>160</v>
       </c>
-      <c r="AQ1" s="547"/>
-      <c r="AR1" s="547"/>
-      <c r="AS1" s="548"/>
-      <c r="AT1" s="579" t="s">
+      <c r="AQ1" s="529"/>
+      <c r="AR1" s="529"/>
+      <c r="AS1" s="530"/>
+      <c r="AT1" s="570" t="s">
         <v>161</v>
       </c>
-      <c r="AU1" s="580"/>
-      <c r="AV1" s="580"/>
-      <c r="AW1" s="580"/>
-      <c r="AX1" s="580"/>
-      <c r="AY1" s="580"/>
-      <c r="AZ1" s="580"/>
-      <c r="BA1" s="580"/>
-      <c r="BB1" s="580"/>
-      <c r="BC1" s="580"/>
-      <c r="BD1" s="580"/>
-      <c r="BE1" s="580"/>
-      <c r="BF1" s="580"/>
-      <c r="BG1" s="580"/>
-      <c r="BH1" s="580"/>
-      <c r="BI1" s="580"/>
-      <c r="BJ1" s="580"/>
-      <c r="BK1" s="580"/>
-      <c r="BL1" s="580"/>
-      <c r="BM1" s="580"/>
-      <c r="BN1" s="580"/>
-      <c r="BO1" s="580"/>
-      <c r="BP1" s="580"/>
-      <c r="BQ1" s="580"/>
-      <c r="BR1" s="580"/>
-      <c r="BS1" s="580"/>
-      <c r="BT1" s="580"/>
-      <c r="BU1" s="580"/>
-      <c r="BV1" s="580"/>
-      <c r="BW1" s="567" t="s">
+      <c r="AU1" s="571"/>
+      <c r="AV1" s="571"/>
+      <c r="AW1" s="571"/>
+      <c r="AX1" s="571"/>
+      <c r="AY1" s="571"/>
+      <c r="AZ1" s="571"/>
+      <c r="BA1" s="571"/>
+      <c r="BB1" s="571"/>
+      <c r="BC1" s="571"/>
+      <c r="BD1" s="571"/>
+      <c r="BE1" s="571"/>
+      <c r="BF1" s="571"/>
+      <c r="BG1" s="571"/>
+      <c r="BH1" s="571"/>
+      <c r="BI1" s="571"/>
+      <c r="BJ1" s="571"/>
+      <c r="BK1" s="571"/>
+      <c r="BL1" s="571"/>
+      <c r="BM1" s="571"/>
+      <c r="BN1" s="571"/>
+      <c r="BO1" s="571"/>
+      <c r="BP1" s="571"/>
+      <c r="BQ1" s="571"/>
+      <c r="BR1" s="571"/>
+      <c r="BS1" s="571"/>
+      <c r="BT1" s="571"/>
+      <c r="BU1" s="571"/>
+      <c r="BV1" s="571"/>
+      <c r="BW1" s="568" t="s">
         <v>162</v>
       </c>
-      <c r="BX1" s="562" t="s">
+      <c r="BX1" s="556" t="s">
         <v>163</v>
       </c>
-      <c r="BY1" s="547"/>
-      <c r="BZ1" s="547"/>
-      <c r="CA1" s="548"/>
-      <c r="CB1" s="569" t="s">
+      <c r="BY1" s="529"/>
+      <c r="BZ1" s="529"/>
+      <c r="CA1" s="530"/>
+      <c r="CB1" s="557" t="s">
         <v>52</v>
       </c>
-      <c r="CC1" s="569"/>
-      <c r="CD1" s="569"/>
-      <c r="CE1" s="569"/>
-      <c r="CF1" s="569"/>
-      <c r="CG1" s="569"/>
-      <c r="CH1" s="569"/>
-      <c r="CI1" s="569"/>
-      <c r="CJ1" s="569"/>
-      <c r="CK1" s="569"/>
-      <c r="CL1" s="569"/>
-      <c r="CM1" s="569"/>
+      <c r="CC1" s="557"/>
+      <c r="CD1" s="557"/>
+      <c r="CE1" s="557"/>
+      <c r="CF1" s="557"/>
+      <c r="CG1" s="557"/>
+      <c r="CH1" s="557"/>
+      <c r="CI1" s="557"/>
+      <c r="CJ1" s="557"/>
+      <c r="CK1" s="557"/>
+      <c r="CL1" s="557"/>
+      <c r="CM1" s="557"/>
       <c r="CN1" s="112"/>
-      <c r="CO1" s="570" t="s">
+      <c r="CO1" s="558" t="s">
         <v>58</v>
       </c>
       <c r="CP1" s="517"/>
@@ -7379,7 +7480,7 @@
       <c r="L2" s="117" t="s">
         <v>61</v>
       </c>
-      <c r="M2" s="556"/>
+      <c r="M2" s="572"/>
       <c r="N2" s="118" t="s">
         <v>168</v>
       </c>
@@ -7395,22 +7496,22 @@
       <c r="R2" s="119" t="s">
         <v>171</v>
       </c>
-      <c r="S2" s="571" t="s">
+      <c r="S2" s="559" t="s">
         <v>172</v>
       </c>
-      <c r="T2" s="542"/>
-      <c r="U2" s="572" t="s">
+      <c r="T2" s="524"/>
+      <c r="U2" s="560" t="s">
         <v>68</v>
       </c>
-      <c r="V2" s="572"/>
-      <c r="W2" s="572" t="s">
+      <c r="V2" s="560"/>
+      <c r="W2" s="560" t="s">
         <v>69</v>
       </c>
-      <c r="X2" s="573"/>
-      <c r="Y2" s="563"/>
-      <c r="Z2" s="564"/>
-      <c r="AA2" s="566"/>
-      <c r="AB2" s="568"/>
+      <c r="X2" s="561"/>
+      <c r="Y2" s="550"/>
+      <c r="Z2" s="551"/>
+      <c r="AA2" s="578"/>
+      <c r="AB2" s="569"/>
       <c r="AC2" s="120" t="s">
         <v>173</v>
       </c>
@@ -7423,81 +7524,81 @@
       <c r="AF2" s="120" t="s">
         <v>176</v>
       </c>
-      <c r="AG2" s="574" t="s">
+      <c r="AG2" s="562" t="s">
         <v>177</v>
       </c>
-      <c r="AH2" s="554"/>
-      <c r="AI2" s="554" t="s">
+      <c r="AH2" s="548"/>
+      <c r="AI2" s="548" t="s">
         <v>178</v>
       </c>
-      <c r="AJ2" s="554"/>
-      <c r="AK2" s="554" t="s">
+      <c r="AJ2" s="548"/>
+      <c r="AK2" s="548" t="s">
         <v>179</v>
       </c>
-      <c r="AL2" s="554"/>
+      <c r="AL2" s="548"/>
       <c r="AM2" s="121" t="s">
         <v>180</v>
       </c>
       <c r="AN2" s="121" t="s">
         <v>181</v>
       </c>
-      <c r="AO2" s="568"/>
-      <c r="AP2" s="563" t="s">
+      <c r="AO2" s="569"/>
+      <c r="AP2" s="550" t="s">
         <v>182</v>
       </c>
-      <c r="AQ2" s="564"/>
+      <c r="AQ2" s="551"/>
       <c r="AR2" s="552" t="s">
         <v>183</v>
       </c>
       <c r="AS2" s="553"/>
-      <c r="AT2" s="554" t="s">
+      <c r="AT2" s="548" t="s">
         <v>184</v>
       </c>
-      <c r="AU2" s="554"/>
-      <c r="AV2" s="555" t="s">
+      <c r="AU2" s="548"/>
+      <c r="AV2" s="549" t="s">
         <v>185</v>
       </c>
-      <c r="AW2" s="555"/>
-      <c r="AX2" s="555" t="s">
+      <c r="AW2" s="549"/>
+      <c r="AX2" s="549" t="s">
         <v>186</v>
       </c>
-      <c r="AY2" s="555"/>
+      <c r="AY2" s="549"/>
       <c r="AZ2" s="121" t="s">
         <v>187</v>
       </c>
       <c r="BA2" s="121" t="s">
         <v>188</v>
       </c>
-      <c r="BB2" s="554" t="s">
+      <c r="BB2" s="548" t="s">
         <v>189</v>
       </c>
-      <c r="BC2" s="554"/>
-      <c r="BD2" s="555" t="s">
+      <c r="BC2" s="548"/>
+      <c r="BD2" s="549" t="s">
         <v>190</v>
       </c>
-      <c r="BE2" s="555"/>
-      <c r="BF2" s="555" t="s">
+      <c r="BE2" s="549"/>
+      <c r="BF2" s="549" t="s">
         <v>191</v>
       </c>
-      <c r="BG2" s="555"/>
+      <c r="BG2" s="549"/>
       <c r="BH2" s="121" t="s">
         <v>192</v>
       </c>
       <c r="BI2" s="121" t="s">
         <v>193</v>
       </c>
-      <c r="BJ2" s="554" t="s">
+      <c r="BJ2" s="548" t="s">
         <v>194</v>
       </c>
-      <c r="BK2" s="554"/>
-      <c r="BL2" s="555" t="s">
+      <c r="BK2" s="548"/>
+      <c r="BL2" s="549" t="s">
         <v>195</v>
       </c>
-      <c r="BM2" s="555"/>
-      <c r="BN2" s="555" t="s">
+      <c r="BM2" s="549"/>
+      <c r="BN2" s="549" t="s">
         <v>196</v>
       </c>
-      <c r="BO2" s="555"/>
+      <c r="BO2" s="549"/>
       <c r="BP2" s="121" t="s">
         <v>197</v>
       </c>
@@ -7519,11 +7620,11 @@
       <c r="BV2" s="121" t="s">
         <v>203</v>
       </c>
-      <c r="BW2" s="568"/>
-      <c r="BX2" s="563" t="s">
+      <c r="BW2" s="569"/>
+      <c r="BX2" s="550" t="s">
         <v>182</v>
       </c>
-      <c r="BY2" s="564"/>
+      <c r="BY2" s="551"/>
       <c r="BZ2" s="552" t="s">
         <v>183</v>
       </c>
@@ -7567,22 +7668,22 @@
       <c r="CN2" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="CO2" s="583" t="s">
+      <c r="CO2" s="554" t="s">
         <v>204</v>
       </c>
-      <c r="CP2" s="584"/>
-      <c r="CQ2" s="581" t="s">
+      <c r="CP2" s="555"/>
+      <c r="CQ2" s="546" t="s">
         <v>205</v>
       </c>
-      <c r="CR2" s="581"/>
-      <c r="CS2" s="584" t="s">
+      <c r="CR2" s="546"/>
+      <c r="CS2" s="555" t="s">
         <v>206</v>
       </c>
-      <c r="CT2" s="584"/>
-      <c r="CU2" s="581" t="s">
+      <c r="CT2" s="555"/>
+      <c r="CU2" s="546" t="s">
         <v>207</v>
       </c>
-      <c r="CV2" s="582"/>
+      <c r="CV2" s="547"/>
     </row>
     <row r="3" spans="1:100" ht="27" x14ac:dyDescent="0.25">
       <c r="A3" s="123" t="s">
@@ -12908,18 +13009,16 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="CU2:CV2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CO2:CP2"/>
-    <mergeCell ref="CQ2:CR2"/>
-    <mergeCell ref="CS2:CT2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
     <mergeCell ref="BX1:CA1"/>
     <mergeCell ref="CB1:CM1"/>
     <mergeCell ref="CO1:CV1"/>
@@ -12936,16 +13035,18 @@
     <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="AT1:BV1"/>
     <mergeCell ref="BW1:BW2"/>
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="CU2:CV2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CO2:CP2"/>
+    <mergeCell ref="CQ2:CR2"/>
+    <mergeCell ref="CS2:CT2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12998,8 +13099,8 @@
       <c r="B2" s="236" t="s">
         <v>246</v>
       </c>
-      <c r="C2" s="585"/>
-      <c r="D2" s="585"/>
+      <c r="C2" s="586"/>
+      <c r="D2" s="586"/>
       <c r="E2" s="234"/>
       <c r="F2" s="234"/>
       <c r="G2" s="234"/>
@@ -13124,32 +13225,32 @@
     </row>
     <row r="7" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="233"/>
-      <c r="B7" s="586" t="s">
+      <c r="B7" s="587" t="s">
         <v>250</v>
       </c>
-      <c r="C7" s="586"/>
-      <c r="D7" s="586"/>
+      <c r="C7" s="587"/>
+      <c r="D7" s="587"/>
       <c r="E7" s="234"/>
       <c r="F7" s="234"/>
       <c r="G7" s="234"/>
       <c r="H7" s="234"/>
       <c r="I7" s="234"/>
-      <c r="J7" s="586" t="s">
+      <c r="J7" s="587" t="s">
         <v>251</v>
       </c>
-      <c r="K7" s="586"/>
-      <c r="L7" s="586"/>
+      <c r="K7" s="587"/>
+      <c r="L7" s="587"/>
       <c r="M7" s="234"/>
       <c r="N7" s="234"/>
       <c r="O7" s="234"/>
       <c r="P7" s="235" t="s">
         <v>252</v>
       </c>
-      <c r="Q7" s="586" t="s">
+      <c r="Q7" s="587" t="s">
         <v>251</v>
       </c>
-      <c r="R7" s="586"/>
-      <c r="S7" s="586"/>
+      <c r="R7" s="587"/>
+      <c r="S7" s="587"/>
       <c r="T7" s="234"/>
       <c r="U7" s="248" t="s">
         <v>253</v>
@@ -13183,41 +13284,41 @@
       <c r="B9" s="249" t="s">
         <v>254</v>
       </c>
-      <c r="C9" s="587" t="s">
+      <c r="C9" s="582" t="s">
         <v>255</v>
       </c>
-      <c r="D9" s="588"/>
-      <c r="E9" s="587" t="s">
+      <c r="D9" s="583"/>
+      <c r="E9" s="582" t="s">
         <v>256</v>
       </c>
-      <c r="F9" s="588"/>
+      <c r="F9" s="583"/>
       <c r="G9" s="234"/>
       <c r="H9" s="234"/>
       <c r="I9" s="234"/>
       <c r="J9" s="249" t="s">
         <v>254</v>
       </c>
-      <c r="K9" s="587" t="s">
+      <c r="K9" s="582" t="s">
         <v>255</v>
       </c>
-      <c r="L9" s="588"/>
-      <c r="M9" s="587" t="s">
+      <c r="L9" s="583"/>
+      <c r="M9" s="582" t="s">
         <v>256</v>
       </c>
-      <c r="N9" s="588"/>
+      <c r="N9" s="583"/>
       <c r="O9" s="234"/>
       <c r="P9" s="234"/>
       <c r="Q9" s="249" t="s">
         <v>254</v>
       </c>
-      <c r="R9" s="587" t="s">
+      <c r="R9" s="582" t="s">
         <v>255</v>
       </c>
-      <c r="S9" s="588"/>
-      <c r="T9" s="587" t="s">
+      <c r="S9" s="583"/>
+      <c r="T9" s="582" t="s">
         <v>256</v>
       </c>
-      <c r="U9" s="588"/>
+      <c r="U9" s="583"/>
     </row>
     <row r="10" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="233"/>
@@ -13279,10 +13380,10 @@
       </c>
       <c r="C11" s="254"/>
       <c r="D11" s="254"/>
-      <c r="E11" s="589" t="s">
+      <c r="E11" s="579" t="s">
         <v>261</v>
       </c>
-      <c r="F11" s="590"/>
+      <c r="F11" s="580"/>
       <c r="G11" s="255"/>
       <c r="H11" s="255"/>
       <c r="I11" s="255"/>
@@ -13291,10 +13392,10 @@
       </c>
       <c r="K11" s="234"/>
       <c r="L11" s="234"/>
-      <c r="M11" s="592" t="s">
+      <c r="M11" s="584" t="s">
         <v>261</v>
       </c>
-      <c r="N11" s="593"/>
+      <c r="N11" s="585"/>
       <c r="O11" s="255"/>
       <c r="P11" s="255"/>
       <c r="Q11" s="253" t="s">
@@ -13302,10 +13403,10 @@
       </c>
       <c r="R11" s="254"/>
       <c r="S11" s="254"/>
-      <c r="T11" s="589" t="s">
+      <c r="T11" s="579" t="s">
         <v>261</v>
       </c>
-      <c r="U11" s="590"/>
+      <c r="U11" s="580"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="233"/>
@@ -13540,10 +13641,10 @@
       </c>
       <c r="C20" s="292"/>
       <c r="D20" s="292"/>
-      <c r="E20" s="589" t="s">
+      <c r="E20" s="579" t="s">
         <v>270</v>
       </c>
-      <c r="F20" s="590"/>
+      <c r="F20" s="580"/>
       <c r="G20" s="269"/>
       <c r="H20" s="269"/>
       <c r="I20" s="234"/>
@@ -13552,10 +13653,10 @@
       </c>
       <c r="K20" s="292"/>
       <c r="L20" s="292"/>
-      <c r="M20" s="589" t="s">
+      <c r="M20" s="579" t="s">
         <v>270</v>
       </c>
-      <c r="N20" s="590"/>
+      <c r="N20" s="580"/>
       <c r="O20" s="282"/>
       <c r="P20" s="282"/>
       <c r="Q20" s="253" t="s">
@@ -13563,10 +13664,10 @@
       </c>
       <c r="R20" s="292"/>
       <c r="S20" s="292"/>
-      <c r="T20" s="589" t="s">
+      <c r="T20" s="579" t="s">
         <v>270</v>
       </c>
-      <c r="U20" s="590"/>
+      <c r="U20" s="580"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="233"/>
@@ -13830,10 +13931,10 @@
       </c>
       <c r="C30" s="292"/>
       <c r="D30" s="292"/>
-      <c r="E30" s="589" t="s">
+      <c r="E30" s="579" t="s">
         <v>270</v>
       </c>
-      <c r="F30" s="590"/>
+      <c r="F30" s="580"/>
       <c r="G30" s="269"/>
       <c r="H30" s="269"/>
       <c r="I30" s="234"/>
@@ -13842,10 +13943,10 @@
       </c>
       <c r="K30" s="292"/>
       <c r="L30" s="292"/>
-      <c r="M30" s="589" t="s">
+      <c r="M30" s="579" t="s">
         <v>270</v>
       </c>
-      <c r="N30" s="590"/>
+      <c r="N30" s="580"/>
       <c r="O30" s="282"/>
       <c r="P30" s="282"/>
       <c r="Q30" s="253" t="s">
@@ -13853,10 +13954,10 @@
       </c>
       <c r="R30" s="292"/>
       <c r="S30" s="292"/>
-      <c r="T30" s="589" t="s">
+      <c r="T30" s="579" t="s">
         <v>270</v>
       </c>
-      <c r="U30" s="590"/>
+      <c r="U30" s="580"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="308"/>
@@ -14179,11 +14280,11 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="233"/>
-      <c r="B42" s="591"/>
-      <c r="C42" s="591"/>
-      <c r="D42" s="591"/>
-      <c r="E42" s="591"/>
-      <c r="F42" s="591"/>
+      <c r="B42" s="581"/>
+      <c r="C42" s="581"/>
+      <c r="D42" s="581"/>
+      <c r="E42" s="581"/>
+      <c r="F42" s="581"/>
       <c r="G42" s="282"/>
       <c r="H42" s="234"/>
       <c r="I42" s="282"/>
@@ -14327,6 +14428,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="R9:S9"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="T30:U30"/>
@@ -14338,15 +14448,6 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="T20:U20"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="R9:S9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14378,8 +14479,8 @@
       <c r="B3" s="335" t="s">
         <v>246</v>
       </c>
-      <c r="C3" s="594"/>
-      <c r="D3" s="594"/>
+      <c r="C3" s="588"/>
+      <c r="D3" s="588"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C4" s="336"/>
@@ -14412,10 +14513,10 @@
       <c r="D10" s="344" t="s">
         <v>290</v>
       </c>
-      <c r="E10" s="595" t="s">
+      <c r="E10" s="589" t="s">
         <v>291</v>
       </c>
-      <c r="F10" s="596"/>
+      <c r="F10" s="590"/>
     </row>
     <row r="11" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="345" t="s">
@@ -14564,10 +14665,10 @@
       <c r="D30" s="379" t="s">
         <v>290</v>
       </c>
-      <c r="E30" s="595" t="s">
+      <c r="E30" s="589" t="s">
         <v>291</v>
       </c>
-      <c r="F30" s="596"/>
+      <c r="F30" s="590"/>
     </row>
     <row r="31" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="345" t="s">
@@ -14713,10 +14814,10 @@
       <c r="D49" s="379" t="s">
         <v>290</v>
       </c>
-      <c r="E49" s="595" t="s">
+      <c r="E49" s="589" t="s">
         <v>291</v>
       </c>
-      <c r="F49" s="596"/>
+      <c r="F49" s="590"/>
     </row>
     <row r="50" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="345" t="s">
@@ -14880,8 +14981,8 @@
       </c>
       <c r="C2" s="236"/>
       <c r="D2" s="236"/>
-      <c r="E2" s="585"/>
-      <c r="F2" s="585"/>
+      <c r="E2" s="586"/>
+      <c r="F2" s="586"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="235"/>
@@ -14913,13 +15014,13 @@
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="233"/>
-      <c r="B6" s="586" t="s">
+      <c r="B6" s="587" t="s">
         <v>303</v>
       </c>
-      <c r="C6" s="586"/>
-      <c r="D6" s="586"/>
-      <c r="E6" s="586"/>
-      <c r="F6" s="586"/>
+      <c r="C6" s="587"/>
+      <c r="D6" s="587"/>
+      <c r="E6" s="587"/>
+      <c r="F6" s="587"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="233"/>
@@ -14934,14 +15035,14 @@
       <c r="B8" s="382" t="s">
         <v>254</v>
       </c>
-      <c r="C8" s="597" t="s">
+      <c r="C8" s="591" t="s">
         <v>255</v>
       </c>
-      <c r="D8" s="597"/>
-      <c r="E8" s="597" t="s">
+      <c r="D8" s="591"/>
+      <c r="E8" s="591" t="s">
         <v>256</v>
       </c>
-      <c r="F8" s="598"/>
+      <c r="F8" s="592"/>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="233"/>
@@ -14996,8 +15097,8 @@
       <c r="B13" s="271"/>
       <c r="C13" s="398"/>
       <c r="D13" s="398"/>
-      <c r="E13" s="599"/>
-      <c r="F13" s="600"/>
+      <c r="E13" s="593"/>
+      <c r="F13" s="594"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="386"/>
@@ -15077,11 +15178,11 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="233"/>
-      <c r="B22" s="591"/>
-      <c r="C22" s="591"/>
-      <c r="D22" s="591"/>
-      <c r="E22" s="591"/>
-      <c r="F22" s="591"/>
+      <c r="B22" s="581"/>
+      <c r="C22" s="581"/>
+      <c r="D22" s="581"/>
+      <c r="E22" s="581"/>
+      <c r="F22" s="581"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="233"/>
@@ -15145,13 +15246,13 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:14" ht="51" x14ac:dyDescent="0.25">
-      <c r="B2" s="601" t="s">
+      <c r="B2" s="595" t="s">
         <v>310</v>
       </c>
-      <c r="C2" s="602" t="s">
+      <c r="C2" s="596" t="s">
         <v>311</v>
       </c>
-      <c r="D2" s="602" t="s">
+      <c r="D2" s="596" t="s">
         <v>166</v>
       </c>
       <c r="E2" s="412" t="s">
@@ -15186,9 +15287,9 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="601"/>
-      <c r="C3" s="603"/>
-      <c r="D3" s="603"/>
+      <c r="B3" s="595"/>
+      <c r="C3" s="597"/>
+      <c r="D3" s="597"/>
       <c r="E3" s="414" t="s">
         <v>320</v>
       </c>
@@ -15221,7 +15322,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="604" t="s">
+      <c r="B4" s="598" t="s">
         <v>323</v>
       </c>
       <c r="C4" s="416" t="s">
@@ -15240,7 +15341,7 @@
       <c r="N4" s="418"/>
     </row>
     <row r="5" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="604"/>
+      <c r="B5" s="598"/>
       <c r="C5" s="416" t="s">
         <v>63</v>
       </c>
@@ -15257,7 +15358,7 @@
       <c r="N5" s="418"/>
     </row>
     <row r="6" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="605"/>
+      <c r="B6" s="599"/>
       <c r="C6" s="419" t="s">
         <v>313</v>
       </c>
@@ -15305,108 +15406,123 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L4"/>
+      <selection sqref="A1:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="12" max="12" width="37.42578125" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="606" t="s">
+      <c r="A1" s="619" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="607"/>
-      <c r="C1" s="608"/>
-      <c r="D1" s="609" t="s">
+      <c r="B1" s="620"/>
+      <c r="C1" s="600"/>
+      <c r="D1" s="621" t="s">
         <v>325</v>
       </c>
-      <c r="E1" s="609"/>
-      <c r="F1" s="610"/>
+      <c r="E1" s="621"/>
+      <c r="F1" s="601"/>
       <c r="G1" s="429" t="s">
         <v>326</v>
       </c>
-      <c r="H1" s="430"/>
-      <c r="I1" s="430"/>
-      <c r="J1" s="430"/>
-      <c r="K1" s="431"/>
-      <c r="L1" s="611" t="s">
+      <c r="H1" s="622"/>
+      <c r="I1" s="622"/>
+      <c r="J1" s="622"/>
+      <c r="K1" s="430"/>
+      <c r="L1" s="602" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="432" t="s">
+      <c r="A2" s="431" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="433" t="s">
+      <c r="B2" s="432" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="434" t="s">
+      <c r="C2" s="433" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="435" t="s">
+      <c r="D2" s="434" t="s">
         <v>328</v>
       </c>
-      <c r="E2" s="436" t="s">
+      <c r="E2" s="435" t="s">
         <v>294</v>
       </c>
-      <c r="F2" s="437" t="s">
+      <c r="F2" s="436" t="s">
         <v>329</v>
       </c>
-      <c r="G2" s="438">
+      <c r="G2" s="437">
         <v>0</v>
       </c>
-      <c r="H2" s="438">
+      <c r="H2" s="437">
         <v>1</v>
       </c>
-      <c r="I2" s="438">
+      <c r="I2" s="437">
         <v>2</v>
       </c>
-      <c r="J2" s="439" t="s">
+      <c r="J2" s="438" t="s">
         <v>330</v>
       </c>
-      <c r="K2" s="440" t="s">
+      <c r="K2" s="439" t="s">
         <v>331</v>
       </c>
-      <c r="L2" s="612"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="441"/>
-      <c r="B3" s="442"/>
-      <c r="C3" s="443" t="s">
+      <c r="L2" s="603"/>
+    </row>
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="440"/>
+      <c r="B3" s="441"/>
+      <c r="C3" s="442" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="613" t="s">
+      <c r="D3" s="604" t="s">
         <v>332</v>
       </c>
-      <c r="E3" s="614"/>
-      <c r="F3" s="615"/>
-      <c r="G3" s="616" t="s">
+      <c r="E3" s="605"/>
+      <c r="F3" s="606"/>
+      <c r="G3" s="607" t="s">
         <v>332</v>
       </c>
-      <c r="H3" s="617"/>
-      <c r="I3" s="617"/>
-      <c r="J3" s="617"/>
-      <c r="K3" s="618"/>
-      <c r="L3" s="612"/>
+      <c r="H3" s="608"/>
+      <c r="I3" s="608"/>
+      <c r="J3" s="608"/>
+      <c r="K3" s="609"/>
+      <c r="L3" s="603"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="444"/>
-      <c r="B4" s="445"/>
-      <c r="C4" s="446"/>
-      <c r="D4" s="447"/>
-      <c r="E4" s="445"/>
-      <c r="F4" s="447"/>
-      <c r="G4" s="445"/>
-      <c r="H4" s="445"/>
-      <c r="I4" s="445"/>
-      <c r="J4" s="445"/>
-      <c r="K4" s="445"/>
-      <c r="L4" s="448"/>
+      <c r="A4" s="623"/>
+      <c r="B4" s="624"/>
+      <c r="C4" s="625"/>
+      <c r="D4" s="626"/>
+      <c r="E4" s="624"/>
+      <c r="F4" s="624"/>
+      <c r="G4" s="624"/>
+      <c r="H4" s="624"/>
+      <c r="I4" s="624"/>
+      <c r="J4" s="624"/>
+      <c r="K4" s="624"/>
+      <c r="L4" s="627"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="628"/>
+      <c r="B5" s="629"/>
+      <c r="C5" s="630"/>
+      <c r="D5" s="631"/>
+      <c r="E5" s="629"/>
+      <c r="F5" s="631"/>
+      <c r="G5" s="629"/>
+      <c r="H5" s="629"/>
+      <c r="I5" s="629"/>
+      <c r="J5" s="629"/>
+      <c r="K5" s="629"/>
+      <c r="L5" s="632"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -15431,106 +15547,106 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="511" t="s">
+      <c r="A1" s="534" t="s">
         <v>333</v>
       </c>
-      <c r="B1" s="512"/>
-      <c r="C1" s="512"/>
-      <c r="D1" s="512"/>
-      <c r="E1" s="449"/>
-      <c r="F1" s="624" t="s">
+      <c r="B1" s="535"/>
+      <c r="C1" s="535"/>
+      <c r="D1" s="535"/>
+      <c r="E1" s="443"/>
+      <c r="F1" s="615" t="s">
         <v>155</v>
       </c>
-      <c r="G1" s="625"/>
-      <c r="H1" s="625"/>
-      <c r="I1" s="450"/>
-      <c r="J1" s="451"/>
-      <c r="K1" s="450"/>
-      <c r="L1" s="452"/>
-      <c r="M1" s="619" t="s">
+      <c r="G1" s="616"/>
+      <c r="H1" s="616"/>
+      <c r="I1" s="444"/>
+      <c r="J1" s="445"/>
+      <c r="K1" s="444"/>
+      <c r="L1" s="446"/>
+      <c r="M1" s="610" t="s">
         <v>334</v>
       </c>
-      <c r="N1" s="453"/>
-      <c r="O1" s="450" t="s">
+      <c r="N1" s="447"/>
+      <c r="O1" s="444" t="s">
         <v>335</v>
       </c>
-      <c r="P1" s="451"/>
-      <c r="Q1" s="450"/>
-      <c r="R1" s="451"/>
-      <c r="S1" s="450"/>
-      <c r="T1" s="452"/>
-      <c r="U1" s="619" t="s">
+      <c r="P1" s="445"/>
+      <c r="Q1" s="444"/>
+      <c r="R1" s="445"/>
+      <c r="S1" s="444"/>
+      <c r="T1" s="446"/>
+      <c r="U1" s="610" t="s">
         <v>336</v>
       </c>
-      <c r="V1" s="453"/>
-      <c r="W1" s="626" t="s">
+      <c r="V1" s="447"/>
+      <c r="W1" s="617" t="s">
         <v>337</v>
       </c>
-      <c r="X1" s="626"/>
-      <c r="Y1" s="626"/>
-      <c r="Z1" s="626"/>
-      <c r="AA1" s="626"/>
-      <c r="AB1" s="627"/>
-      <c r="AC1" s="619" t="s">
+      <c r="X1" s="617"/>
+      <c r="Y1" s="617"/>
+      <c r="Z1" s="617"/>
+      <c r="AA1" s="617"/>
+      <c r="AB1" s="618"/>
+      <c r="AC1" s="610" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="36" x14ac:dyDescent="0.25">
-      <c r="A2" s="454" t="s">
+      <c r="A2" s="448" t="s">
         <v>166</v>
       </c>
-      <c r="B2" s="455" t="s">
+      <c r="B2" s="449" t="s">
         <v>339</v>
       </c>
-      <c r="C2" s="455" t="s">
+      <c r="C2" s="449" t="s">
         <v>340</v>
       </c>
-      <c r="D2" s="621" t="s">
+      <c r="D2" s="612" t="s">
         <v>341</v>
       </c>
-      <c r="E2" s="621"/>
-      <c r="F2" s="456"/>
-      <c r="G2" s="622" t="s">
+      <c r="E2" s="612"/>
+      <c r="F2" s="450"/>
+      <c r="G2" s="613" t="s">
         <v>177</v>
       </c>
-      <c r="H2" s="622"/>
-      <c r="I2" s="622" t="s">
+      <c r="H2" s="613"/>
+      <c r="I2" s="613" t="s">
         <v>178</v>
       </c>
-      <c r="J2" s="622"/>
-      <c r="K2" s="622" t="s">
+      <c r="J2" s="613"/>
+      <c r="K2" s="613" t="s">
         <v>179</v>
       </c>
-      <c r="L2" s="623"/>
-      <c r="M2" s="620"/>
-      <c r="N2" s="457"/>
-      <c r="O2" s="622" t="s">
+      <c r="L2" s="614"/>
+      <c r="M2" s="611"/>
+      <c r="N2" s="451"/>
+      <c r="O2" s="613" t="s">
         <v>177</v>
       </c>
-      <c r="P2" s="622"/>
-      <c r="Q2" s="622" t="s">
+      <c r="P2" s="613"/>
+      <c r="Q2" s="613" t="s">
         <v>178</v>
       </c>
-      <c r="R2" s="622"/>
-      <c r="S2" s="622" t="s">
+      <c r="R2" s="613"/>
+      <c r="S2" s="613" t="s">
         <v>179</v>
       </c>
-      <c r="T2" s="623"/>
-      <c r="U2" s="620"/>
-      <c r="V2" s="457"/>
-      <c r="W2" s="622" t="s">
+      <c r="T2" s="614"/>
+      <c r="U2" s="611"/>
+      <c r="V2" s="451"/>
+      <c r="W2" s="613" t="s">
         <v>177</v>
       </c>
-      <c r="X2" s="622"/>
-      <c r="Y2" s="622" t="s">
+      <c r="X2" s="613"/>
+      <c r="Y2" s="613" t="s">
         <v>178</v>
       </c>
-      <c r="Z2" s="622"/>
-      <c r="AA2" s="622" t="s">
+      <c r="Z2" s="613"/>
+      <c r="AA2" s="613" t="s">
         <v>179</v>
       </c>
-      <c r="AB2" s="623"/>
-      <c r="AC2" s="620"/>
+      <c r="AB2" s="614"/>
+      <c r="AC2" s="611"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
@@ -15548,100 +15664,100 @@
       <c r="E3" s="125" t="s">
         <v>135</v>
       </c>
-      <c r="F3" s="458" t="s">
+      <c r="F3" s="452" t="s">
         <v>343</v>
       </c>
-      <c r="G3" s="459" t="s">
+      <c r="G3" s="453" t="s">
         <v>342</v>
       </c>
-      <c r="H3" s="460" t="s">
+      <c r="H3" s="454" t="s">
         <v>134</v>
       </c>
-      <c r="I3" s="461" t="s">
+      <c r="I3" s="455" t="s">
         <v>342</v>
       </c>
-      <c r="J3" s="460" t="s">
+      <c r="J3" s="454" t="s">
         <v>134</v>
       </c>
-      <c r="K3" s="461" t="s">
+      <c r="K3" s="455" t="s">
         <v>342</v>
       </c>
-      <c r="L3" s="462" t="s">
+      <c r="L3" s="456" t="s">
         <v>134</v>
       </c>
-      <c r="M3" s="463" t="s">
+      <c r="M3" s="457" t="s">
         <v>344</v>
       </c>
-      <c r="N3" s="458" t="s">
+      <c r="N3" s="452" t="s">
         <v>343</v>
       </c>
-      <c r="O3" s="459" t="s">
+      <c r="O3" s="453" t="s">
         <v>342</v>
       </c>
-      <c r="P3" s="460" t="s">
+      <c r="P3" s="454" t="s">
         <v>134</v>
       </c>
-      <c r="Q3" s="461" t="s">
+      <c r="Q3" s="455" t="s">
         <v>342</v>
       </c>
-      <c r="R3" s="460" t="s">
+      <c r="R3" s="454" t="s">
         <v>134</v>
       </c>
-      <c r="S3" s="461" t="s">
+      <c r="S3" s="455" t="s">
         <v>342</v>
       </c>
-      <c r="T3" s="462" t="s">
+      <c r="T3" s="456" t="s">
         <v>134</v>
       </c>
-      <c r="U3" s="463" t="s">
+      <c r="U3" s="457" t="s">
         <v>344</v>
       </c>
-      <c r="V3" s="458" t="s">
+      <c r="V3" s="452" t="s">
         <v>343</v>
       </c>
-      <c r="W3" s="461" t="s">
+      <c r="W3" s="455" t="s">
         <v>342</v>
       </c>
-      <c r="X3" s="460" t="s">
+      <c r="X3" s="454" t="s">
         <v>134</v>
       </c>
-      <c r="Y3" s="461" t="s">
+      <c r="Y3" s="455" t="s">
         <v>342</v>
       </c>
-      <c r="Z3" s="460" t="s">
+      <c r="Z3" s="454" t="s">
         <v>134</v>
       </c>
-      <c r="AA3" s="461" t="s">
+      <c r="AA3" s="455" t="s">
         <v>342</v>
       </c>
-      <c r="AB3" s="462" t="s">
+      <c r="AB3" s="456" t="s">
         <v>134</v>
       </c>
-      <c r="AC3" s="463" t="s">
+      <c r="AC3" s="457" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="156"/>
-      <c r="B4" s="464"/>
-      <c r="C4" s="464"/>
-      <c r="D4" s="464"/>
-      <c r="E4" s="464"/>
-      <c r="F4" s="464"/>
-      <c r="H4" s="464"/>
-      <c r="J4" s="464"/>
-      <c r="L4" s="464"/>
-      <c r="M4" s="464"/>
-      <c r="N4" s="464"/>
-      <c r="P4" s="464"/>
-      <c r="R4" s="464"/>
-      <c r="T4" s="464"/>
-      <c r="U4" s="464"/>
-      <c r="V4" s="464"/>
-      <c r="X4" s="464"/>
-      <c r="Z4" s="464"/>
-      <c r="AB4" s="464"/>
-      <c r="AC4" s="464"/>
+      <c r="B4" s="458"/>
+      <c r="C4" s="458"/>
+      <c r="D4" s="458"/>
+      <c r="E4" s="458"/>
+      <c r="F4" s="458"/>
+      <c r="H4" s="458"/>
+      <c r="J4" s="458"/>
+      <c r="L4" s="458"/>
+      <c r="M4" s="458"/>
+      <c r="N4" s="458"/>
+      <c r="P4" s="458"/>
+      <c r="R4" s="458"/>
+      <c r="T4" s="458"/>
+      <c r="U4" s="458"/>
+      <c r="V4" s="458"/>
+      <c r="X4" s="458"/>
+      <c r="Z4" s="458"/>
+      <c r="AB4" s="458"/>
+      <c r="AC4" s="458"/>
     </row>
   </sheetData>
   <mergeCells count="16">

</xml_diff>

<commit_message>
add new sheet on register, remove agglo and uwwtp with staus = 1 from map pages, correction error
</commit_message>
<xml_diff>
--- a/uwwtd website/sites/all/modules/uwwtd/model/2015_register_model_20151102_2.xlsx
+++ b/uwwtd website/sites/all/modules/uwwtd/model/2015_register_model_20151102_2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e.vincent\Documents\boulot\__SIFFextent\tmp\11\model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e.vincent\Documents\boulot\__SIFFextent\tmp\15\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7440" tabRatio="868" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7440" tabRatio="868" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Sensitive Areas_reference 2012" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="388">
   <si>
     <t>Sensitive areas reported for reference date</t>
   </si>
@@ -1566,6 +1566,24 @@
       </rPr>
       <t>reported under the previous reporting, but not anymore</t>
     </r>
+  </si>
+  <si>
+    <t>Size of Agglomeration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reference year </t>
+  </si>
+  <si>
+    <t>load generated in p.e.</t>
+  </si>
+  <si>
+    <t>2000-10000</t>
+  </si>
+  <si>
+    <t>10001-100000</t>
+  </si>
+  <si>
+    <t>&gt;100 000</t>
   </si>
 </sst>
 </file>
@@ -3260,7 +3278,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="633">
+  <cellXfs count="641">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4492,6 +4510,31 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="59" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="62" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="63" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="63" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="65" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="66" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="66" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4502,6 +4545,48 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="6" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="7" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="7" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4538,12 +4623,6 @@
     <xf numFmtId="3" fontId="11" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="17" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -4589,41 +4668,92 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="33" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="33" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="17" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="12" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="20" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="11" fillId="6" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="7" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="7" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="33" fillId="23" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="33" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="30" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="12" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="33" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -4631,97 +4761,22 @@
     <xf numFmtId="3" fontId="33" fillId="13" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="33" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="33" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="33" fillId="13" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="33" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="30" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="33" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="33" fillId="23" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="33" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="30" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="12" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="20" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="12" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="51" fillId="30" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4733,23 +4788,11 @@
     <xf numFmtId="0" fontId="63" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="51" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="51" fillId="30" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="30" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="65" fillId="32" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4785,7 +4828,16 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="35" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="59" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="18" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4840,40 +4892,24 @@
     <xf numFmtId="3" fontId="13" fillId="12" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="59" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="59" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="62" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="63" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="63" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="65" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="66" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="66" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Hyperlink 2" xfId="10"/>
@@ -5371,54 +5407,54 @@
       <c r="AR3" s="5"/>
     </row>
     <row r="4" spans="1:44" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="501" t="s">
+      <c r="A4" s="512" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="502"/>
-      <c r="C4" s="502"/>
-      <c r="D4" s="502"/>
-      <c r="E4" s="503"/>
-      <c r="F4" s="503"/>
-      <c r="G4" s="503"/>
-      <c r="H4" s="503"/>
-      <c r="I4" s="503"/>
-      <c r="J4" s="503"/>
-      <c r="K4" s="503"/>
-      <c r="L4" s="503"/>
-      <c r="M4" s="503"/>
-      <c r="N4" s="503"/>
-      <c r="O4" s="503"/>
-      <c r="P4" s="503"/>
-      <c r="Q4" s="503"/>
-      <c r="R4" s="503"/>
-      <c r="S4" s="503"/>
-      <c r="T4" s="503"/>
-      <c r="U4" s="503"/>
-      <c r="V4" s="503"/>
-      <c r="W4" s="503"/>
-      <c r="X4" s="503"/>
-      <c r="Y4" s="503"/>
-      <c r="Z4" s="503"/>
-      <c r="AA4" s="503"/>
-      <c r="AB4" s="503"/>
-      <c r="AC4" s="503"/>
-      <c r="AD4" s="503"/>
-      <c r="AE4" s="503"/>
-      <c r="AF4" s="503"/>
-      <c r="AG4" s="503"/>
-      <c r="AH4" s="503"/>
-      <c r="AI4" s="503"/>
-      <c r="AJ4" s="503"/>
-      <c r="AK4" s="503"/>
-      <c r="AL4" s="503"/>
-      <c r="AM4" s="503"/>
-      <c r="AN4" s="503"/>
-      <c r="AO4" s="503"/>
-      <c r="AP4" s="503"/>
-      <c r="AQ4" s="504" t="s">
+      <c r="B4" s="513"/>
+      <c r="C4" s="513"/>
+      <c r="D4" s="513"/>
+      <c r="E4" s="514"/>
+      <c r="F4" s="514"/>
+      <c r="G4" s="514"/>
+      <c r="H4" s="514"/>
+      <c r="I4" s="514"/>
+      <c r="J4" s="514"/>
+      <c r="K4" s="514"/>
+      <c r="L4" s="514"/>
+      <c r="M4" s="514"/>
+      <c r="N4" s="514"/>
+      <c r="O4" s="514"/>
+      <c r="P4" s="514"/>
+      <c r="Q4" s="514"/>
+      <c r="R4" s="514"/>
+      <c r="S4" s="514"/>
+      <c r="T4" s="514"/>
+      <c r="U4" s="514"/>
+      <c r="V4" s="514"/>
+      <c r="W4" s="514"/>
+      <c r="X4" s="514"/>
+      <c r="Y4" s="514"/>
+      <c r="Z4" s="514"/>
+      <c r="AA4" s="514"/>
+      <c r="AB4" s="514"/>
+      <c r="AC4" s="514"/>
+      <c r="AD4" s="514"/>
+      <c r="AE4" s="514"/>
+      <c r="AF4" s="514"/>
+      <c r="AG4" s="514"/>
+      <c r="AH4" s="514"/>
+      <c r="AI4" s="514"/>
+      <c r="AJ4" s="514"/>
+      <c r="AK4" s="514"/>
+      <c r="AL4" s="514"/>
+      <c r="AM4" s="514"/>
+      <c r="AN4" s="514"/>
+      <c r="AO4" s="514"/>
+      <c r="AP4" s="514"/>
+      <c r="AQ4" s="515" t="s">
         <v>3</v>
       </c>
-      <c r="AR4" s="504"/>
+      <c r="AR4" s="515"/>
     </row>
     <row r="5" spans="1:44" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="498" t="s">
@@ -5765,12 +5801,63 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="633" t="s">
+        <v>382</v>
+      </c>
+      <c r="B3" s="634" t="s">
+        <v>383</v>
+      </c>
+      <c r="C3" s="635"/>
+    </row>
+    <row r="4" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A4" s="636"/>
+      <c r="B4" s="637" t="s">
+        <v>257</v>
+      </c>
+      <c r="C4" s="637" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="638" t="s">
+        <v>385</v>
+      </c>
+      <c r="B5" s="639"/>
+      <c r="C5" s="640"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="638" t="s">
+        <v>386</v>
+      </c>
+      <c r="B6" s="639"/>
+      <c r="C6" s="640"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="638" t="s">
+        <v>387</v>
+      </c>
+      <c r="B7" s="639"/>
+      <c r="C7" s="640"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6024,66 +6111,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:101" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="534" t="s">
+      <c r="A1" s="516" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="535"/>
-      <c r="C1" s="535"/>
-      <c r="D1" s="535"/>
-      <c r="E1" s="535"/>
-      <c r="F1" s="535"/>
-      <c r="G1" s="535"/>
-      <c r="H1" s="536" t="s">
+      <c r="B1" s="517"/>
+      <c r="C1" s="517"/>
+      <c r="D1" s="517"/>
+      <c r="E1" s="517"/>
+      <c r="F1" s="517"/>
+      <c r="G1" s="517"/>
+      <c r="H1" s="518" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="537"/>
-      <c r="J1" s="537"/>
-      <c r="K1" s="537"/>
-      <c r="L1" s="537"/>
-      <c r="M1" s="538"/>
-      <c r="N1" s="539" t="s">
+      <c r="I1" s="519"/>
+      <c r="J1" s="519"/>
+      <c r="K1" s="519"/>
+      <c r="L1" s="519"/>
+      <c r="M1" s="520"/>
+      <c r="N1" s="521" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="517"/>
-      <c r="P1" s="517"/>
-      <c r="Q1" s="517"/>
-      <c r="R1" s="517"/>
-      <c r="S1" s="517"/>
-      <c r="T1" s="518"/>
-      <c r="U1" s="540" t="s">
+      <c r="O1" s="522"/>
+      <c r="P1" s="522"/>
+      <c r="Q1" s="522"/>
+      <c r="R1" s="522"/>
+      <c r="S1" s="522"/>
+      <c r="T1" s="523"/>
+      <c r="U1" s="524" t="s">
         <v>51</v>
       </c>
-      <c r="V1" s="541"/>
-      <c r="W1" s="542"/>
-      <c r="X1" s="542"/>
-      <c r="Y1" s="543"/>
-      <c r="Z1" s="544" t="s">
+      <c r="V1" s="525"/>
+      <c r="W1" s="526"/>
+      <c r="X1" s="526"/>
+      <c r="Y1" s="527"/>
+      <c r="Z1" s="528" t="s">
         <v>52</v>
       </c>
-      <c r="AA1" s="545"/>
-      <c r="AB1" s="545"/>
-      <c r="AC1" s="545"/>
-      <c r="AD1" s="545"/>
-      <c r="AE1" s="545"/>
-      <c r="AF1" s="545"/>
-      <c r="AG1" s="545"/>
-      <c r="AH1" s="545"/>
-      <c r="AI1" s="545"/>
-      <c r="AJ1" s="545"/>
-      <c r="AK1" s="545"/>
-      <c r="AL1" s="545"/>
+      <c r="AA1" s="529"/>
+      <c r="AB1" s="529"/>
+      <c r="AC1" s="529"/>
+      <c r="AD1" s="529"/>
+      <c r="AE1" s="529"/>
+      <c r="AF1" s="529"/>
+      <c r="AG1" s="529"/>
+      <c r="AH1" s="529"/>
+      <c r="AI1" s="529"/>
+      <c r="AJ1" s="529"/>
+      <c r="AK1" s="529"/>
+      <c r="AL1" s="529"/>
       <c r="AM1" s="7"/>
       <c r="AN1" s="8"/>
-      <c r="AO1" s="516" t="s">
+      <c r="AO1" s="541" t="s">
         <v>53</v>
       </c>
-      <c r="AP1" s="517"/>
-      <c r="AQ1" s="517"/>
-      <c r="AR1" s="517"/>
-      <c r="AS1" s="517"/>
-      <c r="AT1" s="517"/>
-      <c r="AU1" s="517"/>
-      <c r="AV1" s="518"/>
+      <c r="AP1" s="522"/>
+      <c r="AQ1" s="522"/>
+      <c r="AR1" s="522"/>
+      <c r="AS1" s="522"/>
+      <c r="AT1" s="522"/>
+      <c r="AU1" s="522"/>
+      <c r="AV1" s="523"/>
       <c r="AW1" s="9"/>
       <c r="AX1" s="10"/>
       <c r="AY1" s="11" t="s">
@@ -6093,62 +6180,62 @@
       <c r="BA1" s="12"/>
       <c r="BB1" s="12"/>
       <c r="BC1" s="12"/>
-      <c r="BD1" s="525" t="s">
+      <c r="BD1" s="548" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="526"/>
-      <c r="BF1" s="526"/>
-      <c r="BG1" s="526"/>
-      <c r="BH1" s="526"/>
-      <c r="BI1" s="527"/>
-      <c r="BJ1" s="528" t="s">
+      <c r="BE1" s="549"/>
+      <c r="BF1" s="549"/>
+      <c r="BG1" s="549"/>
+      <c r="BH1" s="549"/>
+      <c r="BI1" s="550"/>
+      <c r="BJ1" s="551" t="s">
         <v>56</v>
       </c>
-      <c r="BK1" s="529"/>
-      <c r="BL1" s="529"/>
-      <c r="BM1" s="529"/>
-      <c r="BN1" s="529"/>
-      <c r="BO1" s="530"/>
-      <c r="BP1" s="531" t="s">
+      <c r="BK1" s="552"/>
+      <c r="BL1" s="552"/>
+      <c r="BM1" s="552"/>
+      <c r="BN1" s="552"/>
+      <c r="BO1" s="553"/>
+      <c r="BP1" s="554" t="s">
         <v>57</v>
       </c>
-      <c r="BQ1" s="532"/>
-      <c r="BR1" s="532"/>
-      <c r="BS1" s="532"/>
-      <c r="BT1" s="532"/>
-      <c r="BU1" s="532"/>
-      <c r="BV1" s="533"/>
-      <c r="BW1" s="505" t="s">
+      <c r="BQ1" s="555"/>
+      <c r="BR1" s="555"/>
+      <c r="BS1" s="555"/>
+      <c r="BT1" s="555"/>
+      <c r="BU1" s="555"/>
+      <c r="BV1" s="556"/>
+      <c r="BW1" s="530" t="s">
         <v>58</v>
       </c>
-      <c r="BX1" s="506"/>
-      <c r="BY1" s="506"/>
-      <c r="BZ1" s="506"/>
-      <c r="CA1" s="506"/>
-      <c r="CB1" s="506"/>
+      <c r="BX1" s="531"/>
+      <c r="BY1" s="531"/>
+      <c r="BZ1" s="531"/>
+      <c r="CA1" s="531"/>
+      <c r="CB1" s="531"/>
       <c r="CC1" s="8"/>
       <c r="CD1" s="13"/>
-      <c r="CE1" s="507" t="s">
+      <c r="CE1" s="532" t="s">
         <v>59</v>
       </c>
-      <c r="CF1" s="508"/>
-      <c r="CG1" s="508"/>
-      <c r="CH1" s="508"/>
-      <c r="CI1" s="508"/>
-      <c r="CJ1" s="508"/>
-      <c r="CK1" s="508"/>
-      <c r="CL1" s="509"/>
-      <c r="CM1" s="509"/>
-      <c r="CN1" s="509"/>
-      <c r="CO1" s="509"/>
-      <c r="CP1" s="509"/>
-      <c r="CQ1" s="509"/>
-      <c r="CR1" s="509"/>
-      <c r="CS1" s="509"/>
-      <c r="CT1" s="509"/>
-      <c r="CU1" s="509"/>
-      <c r="CV1" s="509"/>
-      <c r="CW1" s="509"/>
+      <c r="CF1" s="533"/>
+      <c r="CG1" s="533"/>
+      <c r="CH1" s="533"/>
+      <c r="CI1" s="533"/>
+      <c r="CJ1" s="533"/>
+      <c r="CK1" s="533"/>
+      <c r="CL1" s="534"/>
+      <c r="CM1" s="534"/>
+      <c r="CN1" s="534"/>
+      <c r="CO1" s="534"/>
+      <c r="CP1" s="534"/>
+      <c r="CQ1" s="534"/>
+      <c r="CR1" s="534"/>
+      <c r="CS1" s="534"/>
+      <c r="CT1" s="534"/>
+      <c r="CU1" s="534"/>
+      <c r="CV1" s="534"/>
+      <c r="CW1" s="534"/>
     </row>
     <row r="2" spans="1:101" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -6172,18 +6259,18 @@
       <c r="G2" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="510" t="s">
+      <c r="H2" s="535" t="s">
         <v>67</v>
       </c>
-      <c r="I2" s="511"/>
-      <c r="J2" s="511" t="s">
+      <c r="I2" s="536"/>
+      <c r="J2" s="536" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="511"/>
-      <c r="L2" s="511" t="s">
+      <c r="K2" s="536"/>
+      <c r="L2" s="536" t="s">
         <v>69</v>
       </c>
-      <c r="M2" s="512"/>
+      <c r="M2" s="537"/>
       <c r="N2" s="16" t="s">
         <v>60</v>
       </c>
@@ -6310,36 +6397,36 @@
       <c r="BC2" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="BD2" s="513" t="s">
+      <c r="BD2" s="538" t="s">
         <v>101</v>
       </c>
-      <c r="BE2" s="514"/>
-      <c r="BF2" s="514"/>
-      <c r="BG2" s="514" t="s">
+      <c r="BE2" s="539"/>
+      <c r="BF2" s="539"/>
+      <c r="BG2" s="539" t="s">
         <v>102</v>
       </c>
-      <c r="BH2" s="514"/>
-      <c r="BI2" s="515"/>
-      <c r="BJ2" s="519" t="s">
+      <c r="BH2" s="539"/>
+      <c r="BI2" s="540"/>
+      <c r="BJ2" s="542" t="s">
         <v>101</v>
       </c>
-      <c r="BK2" s="520"/>
-      <c r="BL2" s="520"/>
-      <c r="BM2" s="520" t="s">
+      <c r="BK2" s="543"/>
+      <c r="BL2" s="543"/>
+      <c r="BM2" s="543" t="s">
         <v>102</v>
       </c>
-      <c r="BN2" s="520"/>
-      <c r="BO2" s="521"/>
-      <c r="BP2" s="522" t="s">
+      <c r="BN2" s="543"/>
+      <c r="BO2" s="544"/>
+      <c r="BP2" s="545" t="s">
         <v>101</v>
       </c>
-      <c r="BQ2" s="523"/>
-      <c r="BR2" s="523"/>
-      <c r="BS2" s="523" t="s">
+      <c r="BQ2" s="546"/>
+      <c r="BR2" s="546"/>
+      <c r="BS2" s="546" t="s">
         <v>102</v>
       </c>
-      <c r="BT2" s="524"/>
-      <c r="BU2" s="524"/>
+      <c r="BT2" s="547"/>
+      <c r="BU2" s="547"/>
       <c r="BV2" s="31" t="s">
         <v>103</v>
       </c>
@@ -7266,11 +7353,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:T1"/>
-    <mergeCell ref="U1:Y1"/>
-    <mergeCell ref="Z1:AL1"/>
     <mergeCell ref="BW1:CB1"/>
     <mergeCell ref="CE1:CW1"/>
     <mergeCell ref="H2:I2"/>
@@ -7286,6 +7368,11 @@
     <mergeCell ref="BD1:BI1"/>
     <mergeCell ref="BJ1:BO1"/>
     <mergeCell ref="BP1:BV1"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:T1"/>
+    <mergeCell ref="U1:Y1"/>
+    <mergeCell ref="Z1:AL1"/>
   </mergeCells>
   <conditionalFormatting sqref="A13:A14 A4:B4">
     <cfRule type="duplicateValues" dxfId="8" priority="1"/>
@@ -7324,124 +7411,124 @@
         <v>150</v>
       </c>
       <c r="L1" s="111"/>
-      <c r="M1" s="572" t="s">
+      <c r="M1" s="561" t="s">
         <v>151</v>
       </c>
-      <c r="N1" s="573" t="s">
+      <c r="N1" s="562" t="s">
         <v>152</v>
       </c>
-      <c r="O1" s="574"/>
-      <c r="P1" s="574"/>
-      <c r="Q1" s="574"/>
-      <c r="R1" s="575" t="s">
+      <c r="O1" s="563"/>
+      <c r="P1" s="563"/>
+      <c r="Q1" s="563"/>
+      <c r="R1" s="564" t="s">
         <v>153</v>
       </c>
-      <c r="S1" s="567"/>
-      <c r="T1" s="567"/>
-      <c r="U1" s="567"/>
-      <c r="V1" s="567"/>
-      <c r="W1" s="567"/>
-      <c r="X1" s="576"/>
-      <c r="Y1" s="556" t="s">
+      <c r="S1" s="565"/>
+      <c r="T1" s="565"/>
+      <c r="U1" s="565"/>
+      <c r="V1" s="565"/>
+      <c r="W1" s="565"/>
+      <c r="X1" s="566"/>
+      <c r="Y1" s="567" t="s">
         <v>154</v>
       </c>
-      <c r="Z1" s="529"/>
-      <c r="AA1" s="577" t="s">
+      <c r="Z1" s="552"/>
+      <c r="AA1" s="570" t="s">
         <v>155</v>
       </c>
-      <c r="AB1" s="568" t="s">
+      <c r="AB1" s="572" t="s">
         <v>156</v>
       </c>
-      <c r="AC1" s="563" t="s">
+      <c r="AC1" s="580" t="s">
         <v>157</v>
       </c>
-      <c r="AD1" s="564"/>
-      <c r="AE1" s="564"/>
-      <c r="AF1" s="565"/>
-      <c r="AG1" s="566" t="s">
+      <c r="AD1" s="581"/>
+      <c r="AE1" s="581"/>
+      <c r="AF1" s="582"/>
+      <c r="AG1" s="583" t="s">
         <v>158</v>
       </c>
-      <c r="AH1" s="567"/>
-      <c r="AI1" s="567"/>
-      <c r="AJ1" s="567"/>
-      <c r="AK1" s="567"/>
-      <c r="AL1" s="567"/>
-      <c r="AM1" s="567"/>
-      <c r="AN1" s="567"/>
-      <c r="AO1" s="568" t="s">
+      <c r="AH1" s="565"/>
+      <c r="AI1" s="565"/>
+      <c r="AJ1" s="565"/>
+      <c r="AK1" s="565"/>
+      <c r="AL1" s="565"/>
+      <c r="AM1" s="565"/>
+      <c r="AN1" s="565"/>
+      <c r="AO1" s="572" t="s">
         <v>159</v>
       </c>
-      <c r="AP1" s="556" t="s">
+      <c r="AP1" s="567" t="s">
         <v>160</v>
       </c>
-      <c r="AQ1" s="529"/>
-      <c r="AR1" s="529"/>
-      <c r="AS1" s="530"/>
-      <c r="AT1" s="570" t="s">
+      <c r="AQ1" s="552"/>
+      <c r="AR1" s="552"/>
+      <c r="AS1" s="553"/>
+      <c r="AT1" s="584" t="s">
         <v>161</v>
       </c>
-      <c r="AU1" s="571"/>
-      <c r="AV1" s="571"/>
-      <c r="AW1" s="571"/>
-      <c r="AX1" s="571"/>
-      <c r="AY1" s="571"/>
-      <c r="AZ1" s="571"/>
-      <c r="BA1" s="571"/>
-      <c r="BB1" s="571"/>
-      <c r="BC1" s="571"/>
-      <c r="BD1" s="571"/>
-      <c r="BE1" s="571"/>
-      <c r="BF1" s="571"/>
-      <c r="BG1" s="571"/>
-      <c r="BH1" s="571"/>
-      <c r="BI1" s="571"/>
-      <c r="BJ1" s="571"/>
-      <c r="BK1" s="571"/>
-      <c r="BL1" s="571"/>
-      <c r="BM1" s="571"/>
-      <c r="BN1" s="571"/>
-      <c r="BO1" s="571"/>
-      <c r="BP1" s="571"/>
-      <c r="BQ1" s="571"/>
-      <c r="BR1" s="571"/>
-      <c r="BS1" s="571"/>
-      <c r="BT1" s="571"/>
-      <c r="BU1" s="571"/>
-      <c r="BV1" s="571"/>
-      <c r="BW1" s="568" t="s">
+      <c r="AU1" s="585"/>
+      <c r="AV1" s="585"/>
+      <c r="AW1" s="585"/>
+      <c r="AX1" s="585"/>
+      <c r="AY1" s="585"/>
+      <c r="AZ1" s="585"/>
+      <c r="BA1" s="585"/>
+      <c r="BB1" s="585"/>
+      <c r="BC1" s="585"/>
+      <c r="BD1" s="585"/>
+      <c r="BE1" s="585"/>
+      <c r="BF1" s="585"/>
+      <c r="BG1" s="585"/>
+      <c r="BH1" s="585"/>
+      <c r="BI1" s="585"/>
+      <c r="BJ1" s="585"/>
+      <c r="BK1" s="585"/>
+      <c r="BL1" s="585"/>
+      <c r="BM1" s="585"/>
+      <c r="BN1" s="585"/>
+      <c r="BO1" s="585"/>
+      <c r="BP1" s="585"/>
+      <c r="BQ1" s="585"/>
+      <c r="BR1" s="585"/>
+      <c r="BS1" s="585"/>
+      <c r="BT1" s="585"/>
+      <c r="BU1" s="585"/>
+      <c r="BV1" s="585"/>
+      <c r="BW1" s="572" t="s">
         <v>162</v>
       </c>
-      <c r="BX1" s="556" t="s">
+      <c r="BX1" s="567" t="s">
         <v>163</v>
       </c>
-      <c r="BY1" s="529"/>
-      <c r="BZ1" s="529"/>
-      <c r="CA1" s="530"/>
-      <c r="CB1" s="557" t="s">
+      <c r="BY1" s="552"/>
+      <c r="BZ1" s="552"/>
+      <c r="CA1" s="553"/>
+      <c r="CB1" s="574" t="s">
         <v>52</v>
       </c>
-      <c r="CC1" s="557"/>
-      <c r="CD1" s="557"/>
-      <c r="CE1" s="557"/>
-      <c r="CF1" s="557"/>
-      <c r="CG1" s="557"/>
-      <c r="CH1" s="557"/>
-      <c r="CI1" s="557"/>
-      <c r="CJ1" s="557"/>
-      <c r="CK1" s="557"/>
-      <c r="CL1" s="557"/>
-      <c r="CM1" s="557"/>
+      <c r="CC1" s="574"/>
+      <c r="CD1" s="574"/>
+      <c r="CE1" s="574"/>
+      <c r="CF1" s="574"/>
+      <c r="CG1" s="574"/>
+      <c r="CH1" s="574"/>
+      <c r="CI1" s="574"/>
+      <c r="CJ1" s="574"/>
+      <c r="CK1" s="574"/>
+      <c r="CL1" s="574"/>
+      <c r="CM1" s="574"/>
       <c r="CN1" s="112"/>
-      <c r="CO1" s="558" t="s">
+      <c r="CO1" s="575" t="s">
         <v>58</v>
       </c>
-      <c r="CP1" s="517"/>
-      <c r="CQ1" s="517"/>
-      <c r="CR1" s="517"/>
-      <c r="CS1" s="517"/>
-      <c r="CT1" s="517"/>
-      <c r="CU1" s="517"/>
-      <c r="CV1" s="518"/>
+      <c r="CP1" s="522"/>
+      <c r="CQ1" s="522"/>
+      <c r="CR1" s="522"/>
+      <c r="CS1" s="522"/>
+      <c r="CT1" s="522"/>
+      <c r="CU1" s="522"/>
+      <c r="CV1" s="523"/>
     </row>
     <row r="2" spans="1:100" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A2" s="113" t="s">
@@ -7480,7 +7567,7 @@
       <c r="L2" s="117" t="s">
         <v>61</v>
       </c>
-      <c r="M2" s="572"/>
+      <c r="M2" s="561"/>
       <c r="N2" s="118" t="s">
         <v>168</v>
       </c>
@@ -7496,22 +7583,22 @@
       <c r="R2" s="119" t="s">
         <v>171</v>
       </c>
-      <c r="S2" s="559" t="s">
+      <c r="S2" s="576" t="s">
         <v>172</v>
       </c>
-      <c r="T2" s="524"/>
-      <c r="U2" s="560" t="s">
+      <c r="T2" s="547"/>
+      <c r="U2" s="577" t="s">
         <v>68</v>
       </c>
-      <c r="V2" s="560"/>
-      <c r="W2" s="560" t="s">
+      <c r="V2" s="577"/>
+      <c r="W2" s="577" t="s">
         <v>69</v>
       </c>
-      <c r="X2" s="561"/>
-      <c r="Y2" s="550"/>
-      <c r="Z2" s="551"/>
-      <c r="AA2" s="578"/>
-      <c r="AB2" s="569"/>
+      <c r="X2" s="578"/>
+      <c r="Y2" s="568"/>
+      <c r="Z2" s="569"/>
+      <c r="AA2" s="571"/>
+      <c r="AB2" s="573"/>
       <c r="AC2" s="120" t="s">
         <v>173</v>
       </c>
@@ -7524,81 +7611,81 @@
       <c r="AF2" s="120" t="s">
         <v>176</v>
       </c>
-      <c r="AG2" s="562" t="s">
+      <c r="AG2" s="579" t="s">
         <v>177</v>
       </c>
-      <c r="AH2" s="548"/>
-      <c r="AI2" s="548" t="s">
+      <c r="AH2" s="559"/>
+      <c r="AI2" s="559" t="s">
         <v>178</v>
       </c>
-      <c r="AJ2" s="548"/>
-      <c r="AK2" s="548" t="s">
+      <c r="AJ2" s="559"/>
+      <c r="AK2" s="559" t="s">
         <v>179</v>
       </c>
-      <c r="AL2" s="548"/>
+      <c r="AL2" s="559"/>
       <c r="AM2" s="121" t="s">
         <v>180</v>
       </c>
       <c r="AN2" s="121" t="s">
         <v>181</v>
       </c>
-      <c r="AO2" s="569"/>
-      <c r="AP2" s="550" t="s">
+      <c r="AO2" s="573"/>
+      <c r="AP2" s="568" t="s">
         <v>182</v>
       </c>
-      <c r="AQ2" s="551"/>
-      <c r="AR2" s="552" t="s">
+      <c r="AQ2" s="569"/>
+      <c r="AR2" s="557" t="s">
         <v>183</v>
       </c>
-      <c r="AS2" s="553"/>
-      <c r="AT2" s="548" t="s">
+      <c r="AS2" s="558"/>
+      <c r="AT2" s="559" t="s">
         <v>184</v>
       </c>
-      <c r="AU2" s="548"/>
-      <c r="AV2" s="549" t="s">
+      <c r="AU2" s="559"/>
+      <c r="AV2" s="560" t="s">
         <v>185</v>
       </c>
-      <c r="AW2" s="549"/>
-      <c r="AX2" s="549" t="s">
+      <c r="AW2" s="560"/>
+      <c r="AX2" s="560" t="s">
         <v>186</v>
       </c>
-      <c r="AY2" s="549"/>
+      <c r="AY2" s="560"/>
       <c r="AZ2" s="121" t="s">
         <v>187</v>
       </c>
       <c r="BA2" s="121" t="s">
         <v>188</v>
       </c>
-      <c r="BB2" s="548" t="s">
+      <c r="BB2" s="559" t="s">
         <v>189</v>
       </c>
-      <c r="BC2" s="548"/>
-      <c r="BD2" s="549" t="s">
+      <c r="BC2" s="559"/>
+      <c r="BD2" s="560" t="s">
         <v>190</v>
       </c>
-      <c r="BE2" s="549"/>
-      <c r="BF2" s="549" t="s">
+      <c r="BE2" s="560"/>
+      <c r="BF2" s="560" t="s">
         <v>191</v>
       </c>
-      <c r="BG2" s="549"/>
+      <c r="BG2" s="560"/>
       <c r="BH2" s="121" t="s">
         <v>192</v>
       </c>
       <c r="BI2" s="121" t="s">
         <v>193</v>
       </c>
-      <c r="BJ2" s="548" t="s">
+      <c r="BJ2" s="559" t="s">
         <v>194</v>
       </c>
-      <c r="BK2" s="548"/>
-      <c r="BL2" s="549" t="s">
+      <c r="BK2" s="559"/>
+      <c r="BL2" s="560" t="s">
         <v>195</v>
       </c>
-      <c r="BM2" s="549"/>
-      <c r="BN2" s="549" t="s">
+      <c r="BM2" s="560"/>
+      <c r="BN2" s="560" t="s">
         <v>196</v>
       </c>
-      <c r="BO2" s="549"/>
+      <c r="BO2" s="560"/>
       <c r="BP2" s="121" t="s">
         <v>197</v>
       </c>
@@ -7620,15 +7707,15 @@
       <c r="BV2" s="121" t="s">
         <v>203</v>
       </c>
-      <c r="BW2" s="569"/>
-      <c r="BX2" s="550" t="s">
+      <c r="BW2" s="573"/>
+      <c r="BX2" s="568" t="s">
         <v>182</v>
       </c>
-      <c r="BY2" s="551"/>
-      <c r="BZ2" s="552" t="s">
+      <c r="BY2" s="569"/>
+      <c r="BZ2" s="557" t="s">
         <v>183</v>
       </c>
-      <c r="CA2" s="553"/>
+      <c r="CA2" s="558"/>
       <c r="CB2" s="24" t="s">
         <v>76</v>
       </c>
@@ -7668,22 +7755,22 @@
       <c r="CN2" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="CO2" s="554" t="s">
+      <c r="CO2" s="588" t="s">
         <v>204</v>
       </c>
-      <c r="CP2" s="555"/>
-      <c r="CQ2" s="546" t="s">
+      <c r="CP2" s="589"/>
+      <c r="CQ2" s="586" t="s">
         <v>205</v>
       </c>
-      <c r="CR2" s="546"/>
-      <c r="CS2" s="555" t="s">
+      <c r="CR2" s="586"/>
+      <c r="CS2" s="589" t="s">
         <v>206</v>
       </c>
-      <c r="CT2" s="555"/>
-      <c r="CU2" s="546" t="s">
+      <c r="CT2" s="589"/>
+      <c r="CU2" s="586" t="s">
         <v>207</v>
       </c>
-      <c r="CV2" s="547"/>
+      <c r="CV2" s="587"/>
     </row>
     <row r="3" spans="1:100" ht="27" x14ac:dyDescent="0.25">
       <c r="A3" s="123" t="s">
@@ -13009,16 +13096,18 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="AR2:AS2"/>
-    <mergeCell ref="AT2:AU2"/>
-    <mergeCell ref="AV2:AW2"/>
-    <mergeCell ref="AX2:AY2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="Y1:Z2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="CU2:CV2"/>
+    <mergeCell ref="BB2:BC2"/>
+    <mergeCell ref="BD2:BE2"/>
+    <mergeCell ref="BF2:BG2"/>
+    <mergeCell ref="BJ2:BK2"/>
+    <mergeCell ref="BL2:BM2"/>
+    <mergeCell ref="BN2:BO2"/>
+    <mergeCell ref="BX2:BY2"/>
+    <mergeCell ref="BZ2:CA2"/>
+    <mergeCell ref="CO2:CP2"/>
+    <mergeCell ref="CQ2:CR2"/>
+    <mergeCell ref="CS2:CT2"/>
     <mergeCell ref="BX1:CA1"/>
     <mergeCell ref="CB1:CM1"/>
     <mergeCell ref="CO1:CV1"/>
@@ -13035,18 +13124,16 @@
     <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="AT1:BV1"/>
     <mergeCell ref="BW1:BW2"/>
-    <mergeCell ref="CU2:CV2"/>
-    <mergeCell ref="BB2:BC2"/>
-    <mergeCell ref="BD2:BE2"/>
-    <mergeCell ref="BF2:BG2"/>
-    <mergeCell ref="BJ2:BK2"/>
-    <mergeCell ref="BL2:BM2"/>
-    <mergeCell ref="BN2:BO2"/>
-    <mergeCell ref="BX2:BY2"/>
-    <mergeCell ref="BZ2:CA2"/>
-    <mergeCell ref="CO2:CP2"/>
-    <mergeCell ref="CQ2:CR2"/>
-    <mergeCell ref="CS2:CT2"/>
+    <mergeCell ref="AR2:AS2"/>
+    <mergeCell ref="AT2:AU2"/>
+    <mergeCell ref="AV2:AW2"/>
+    <mergeCell ref="AX2:AY2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="Y1:Z2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13099,8 +13186,8 @@
       <c r="B2" s="236" t="s">
         <v>246</v>
       </c>
-      <c r="C2" s="586"/>
-      <c r="D2" s="586"/>
+      <c r="C2" s="590"/>
+      <c r="D2" s="590"/>
       <c r="E2" s="234"/>
       <c r="F2" s="234"/>
       <c r="G2" s="234"/>
@@ -13225,32 +13312,32 @@
     </row>
     <row r="7" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="233"/>
-      <c r="B7" s="587" t="s">
+      <c r="B7" s="591" t="s">
         <v>250</v>
       </c>
-      <c r="C7" s="587"/>
-      <c r="D7" s="587"/>
+      <c r="C7" s="591"/>
+      <c r="D7" s="591"/>
       <c r="E7" s="234"/>
       <c r="F7" s="234"/>
       <c r="G7" s="234"/>
       <c r="H7" s="234"/>
       <c r="I7" s="234"/>
-      <c r="J7" s="587" t="s">
+      <c r="J7" s="591" t="s">
         <v>251</v>
       </c>
-      <c r="K7" s="587"/>
-      <c r="L7" s="587"/>
+      <c r="K7" s="591"/>
+      <c r="L7" s="591"/>
       <c r="M7" s="234"/>
       <c r="N7" s="234"/>
       <c r="O7" s="234"/>
       <c r="P7" s="235" t="s">
         <v>252</v>
       </c>
-      <c r="Q7" s="587" t="s">
+      <c r="Q7" s="591" t="s">
         <v>251</v>
       </c>
-      <c r="R7" s="587"/>
-      <c r="S7" s="587"/>
+      <c r="R7" s="591"/>
+      <c r="S7" s="591"/>
       <c r="T7" s="234"/>
       <c r="U7" s="248" t="s">
         <v>253</v>
@@ -13284,41 +13371,41 @@
       <c r="B9" s="249" t="s">
         <v>254</v>
       </c>
-      <c r="C9" s="582" t="s">
+      <c r="C9" s="592" t="s">
         <v>255</v>
       </c>
-      <c r="D9" s="583"/>
-      <c r="E9" s="582" t="s">
+      <c r="D9" s="593"/>
+      <c r="E9" s="592" t="s">
         <v>256</v>
       </c>
-      <c r="F9" s="583"/>
+      <c r="F9" s="593"/>
       <c r="G9" s="234"/>
       <c r="H9" s="234"/>
       <c r="I9" s="234"/>
       <c r="J9" s="249" t="s">
         <v>254</v>
       </c>
-      <c r="K9" s="582" t="s">
+      <c r="K9" s="592" t="s">
         <v>255</v>
       </c>
-      <c r="L9" s="583"/>
-      <c r="M9" s="582" t="s">
+      <c r="L9" s="593"/>
+      <c r="M9" s="592" t="s">
         <v>256</v>
       </c>
-      <c r="N9" s="583"/>
+      <c r="N9" s="593"/>
       <c r="O9" s="234"/>
       <c r="P9" s="234"/>
       <c r="Q9" s="249" t="s">
         <v>254</v>
       </c>
-      <c r="R9" s="582" t="s">
+      <c r="R9" s="592" t="s">
         <v>255</v>
       </c>
-      <c r="S9" s="583"/>
-      <c r="T9" s="582" t="s">
+      <c r="S9" s="593"/>
+      <c r="T9" s="592" t="s">
         <v>256</v>
       </c>
-      <c r="U9" s="583"/>
+      <c r="U9" s="593"/>
     </row>
     <row r="10" spans="1:21" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="233"/>
@@ -13380,10 +13467,10 @@
       </c>
       <c r="C11" s="254"/>
       <c r="D11" s="254"/>
-      <c r="E11" s="579" t="s">
+      <c r="E11" s="594" t="s">
         <v>261</v>
       </c>
-      <c r="F11" s="580"/>
+      <c r="F11" s="595"/>
       <c r="G11" s="255"/>
       <c r="H11" s="255"/>
       <c r="I11" s="255"/>
@@ -13392,10 +13479,10 @@
       </c>
       <c r="K11" s="234"/>
       <c r="L11" s="234"/>
-      <c r="M11" s="584" t="s">
+      <c r="M11" s="597" t="s">
         <v>261</v>
       </c>
-      <c r="N11" s="585"/>
+      <c r="N11" s="598"/>
       <c r="O11" s="255"/>
       <c r="P11" s="255"/>
       <c r="Q11" s="253" t="s">
@@ -13403,10 +13490,10 @@
       </c>
       <c r="R11" s="254"/>
       <c r="S11" s="254"/>
-      <c r="T11" s="579" t="s">
+      <c r="T11" s="594" t="s">
         <v>261</v>
       </c>
-      <c r="U11" s="580"/>
+      <c r="U11" s="595"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="233"/>
@@ -13641,10 +13728,10 @@
       </c>
       <c r="C20" s="292"/>
       <c r="D20" s="292"/>
-      <c r="E20" s="579" t="s">
+      <c r="E20" s="594" t="s">
         <v>270</v>
       </c>
-      <c r="F20" s="580"/>
+      <c r="F20" s="595"/>
       <c r="G20" s="269"/>
       <c r="H20" s="269"/>
       <c r="I20" s="234"/>
@@ -13653,10 +13740,10 @@
       </c>
       <c r="K20" s="292"/>
       <c r="L20" s="292"/>
-      <c r="M20" s="579" t="s">
+      <c r="M20" s="594" t="s">
         <v>270</v>
       </c>
-      <c r="N20" s="580"/>
+      <c r="N20" s="595"/>
       <c r="O20" s="282"/>
       <c r="P20" s="282"/>
       <c r="Q20" s="253" t="s">
@@ -13664,10 +13751,10 @@
       </c>
       <c r="R20" s="292"/>
       <c r="S20" s="292"/>
-      <c r="T20" s="579" t="s">
+      <c r="T20" s="594" t="s">
         <v>270</v>
       </c>
-      <c r="U20" s="580"/>
+      <c r="U20" s="595"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="233"/>
@@ -13756,7 +13843,7 @@
       <c r="T23" s="280"/>
       <c r="U23" s="281"/>
     </row>
-    <row r="24" spans="1:21" ht="24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="36" x14ac:dyDescent="0.25">
       <c r="A24" s="233"/>
       <c r="B24" s="298" t="s">
         <v>272</v>
@@ -13931,10 +14018,10 @@
       </c>
       <c r="C30" s="292"/>
       <c r="D30" s="292"/>
-      <c r="E30" s="579" t="s">
+      <c r="E30" s="594" t="s">
         <v>270</v>
       </c>
-      <c r="F30" s="580"/>
+      <c r="F30" s="595"/>
       <c r="G30" s="269"/>
       <c r="H30" s="269"/>
       <c r="I30" s="234"/>
@@ -13943,10 +14030,10 @@
       </c>
       <c r="K30" s="292"/>
       <c r="L30" s="292"/>
-      <c r="M30" s="579" t="s">
+      <c r="M30" s="594" t="s">
         <v>270</v>
       </c>
-      <c r="N30" s="580"/>
+      <c r="N30" s="595"/>
       <c r="O30" s="282"/>
       <c r="P30" s="282"/>
       <c r="Q30" s="253" t="s">
@@ -13954,10 +14041,10 @@
       </c>
       <c r="R30" s="292"/>
       <c r="S30" s="292"/>
-      <c r="T30" s="579" t="s">
+      <c r="T30" s="594" t="s">
         <v>270</v>
       </c>
-      <c r="U30" s="580"/>
+      <c r="U30" s="595"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="308"/>
@@ -14280,11 +14367,11 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="233"/>
-      <c r="B42" s="581"/>
-      <c r="C42" s="581"/>
-      <c r="D42" s="581"/>
-      <c r="E42" s="581"/>
-      <c r="F42" s="581"/>
+      <c r="B42" s="596"/>
+      <c r="C42" s="596"/>
+      <c r="D42" s="596"/>
+      <c r="E42" s="596"/>
+      <c r="F42" s="596"/>
       <c r="G42" s="282"/>
       <c r="H42" s="234"/>
       <c r="I42" s="282"/>
@@ -14428,15 +14515,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="R9:S9"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="M30:N30"/>
     <mergeCell ref="T30:U30"/>
@@ -14448,6 +14526,15 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="T20:U20"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="R9:S9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14479,8 +14566,8 @@
       <c r="B3" s="335" t="s">
         <v>246</v>
       </c>
-      <c r="C3" s="588"/>
-      <c r="D3" s="588"/>
+      <c r="C3" s="599"/>
+      <c r="D3" s="599"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C4" s="336"/>
@@ -14513,10 +14600,10 @@
       <c r="D10" s="344" t="s">
         <v>290</v>
       </c>
-      <c r="E10" s="589" t="s">
+      <c r="E10" s="600" t="s">
         <v>291</v>
       </c>
-      <c r="F10" s="590"/>
+      <c r="F10" s="601"/>
     </row>
     <row r="11" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="345" t="s">
@@ -14665,10 +14752,10 @@
       <c r="D30" s="379" t="s">
         <v>290</v>
       </c>
-      <c r="E30" s="589" t="s">
+      <c r="E30" s="600" t="s">
         <v>291</v>
       </c>
-      <c r="F30" s="590"/>
+      <c r="F30" s="601"/>
     </row>
     <row r="31" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="345" t="s">
@@ -14814,10 +14901,10 @@
       <c r="D49" s="379" t="s">
         <v>290</v>
       </c>
-      <c r="E49" s="589" t="s">
+      <c r="E49" s="600" t="s">
         <v>291</v>
       </c>
-      <c r="F49" s="590"/>
+      <c r="F49" s="601"/>
     </row>
     <row r="50" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="345" t="s">
@@ -14981,8 +15068,8 @@
       </c>
       <c r="C2" s="236"/>
       <c r="D2" s="236"/>
-      <c r="E2" s="586"/>
-      <c r="F2" s="586"/>
+      <c r="E2" s="590"/>
+      <c r="F2" s="590"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="235"/>
@@ -15014,13 +15101,13 @@
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="233"/>
-      <c r="B6" s="587" t="s">
+      <c r="B6" s="591" t="s">
         <v>303</v>
       </c>
-      <c r="C6" s="587"/>
-      <c r="D6" s="587"/>
-      <c r="E6" s="587"/>
-      <c r="F6" s="587"/>
+      <c r="C6" s="591"/>
+      <c r="D6" s="591"/>
+      <c r="E6" s="591"/>
+      <c r="F6" s="591"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="233"/>
@@ -15035,14 +15122,14 @@
       <c r="B8" s="382" t="s">
         <v>254</v>
       </c>
-      <c r="C8" s="591" t="s">
+      <c r="C8" s="602" t="s">
         <v>255</v>
       </c>
-      <c r="D8" s="591"/>
-      <c r="E8" s="591" t="s">
+      <c r="D8" s="602"/>
+      <c r="E8" s="602" t="s">
         <v>256</v>
       </c>
-      <c r="F8" s="592"/>
+      <c r="F8" s="603"/>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="233"/>
@@ -15097,8 +15184,8 @@
       <c r="B13" s="271"/>
       <c r="C13" s="398"/>
       <c r="D13" s="398"/>
-      <c r="E13" s="593"/>
-      <c r="F13" s="594"/>
+      <c r="E13" s="604"/>
+      <c r="F13" s="605"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="386"/>
@@ -15178,11 +15265,11 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="233"/>
-      <c r="B22" s="581"/>
-      <c r="C22" s="581"/>
-      <c r="D22" s="581"/>
-      <c r="E22" s="581"/>
-      <c r="F22" s="581"/>
+      <c r="B22" s="596"/>
+      <c r="C22" s="596"/>
+      <c r="D22" s="596"/>
+      <c r="E22" s="596"/>
+      <c r="F22" s="596"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="233"/>
@@ -15246,13 +15333,13 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:14" ht="51" x14ac:dyDescent="0.25">
-      <c r="B2" s="595" t="s">
+      <c r="B2" s="606" t="s">
         <v>310</v>
       </c>
-      <c r="C2" s="596" t="s">
+      <c r="C2" s="607" t="s">
         <v>311</v>
       </c>
-      <c r="D2" s="596" t="s">
+      <c r="D2" s="607" t="s">
         <v>166</v>
       </c>
       <c r="E2" s="412" t="s">
@@ -15287,9 +15374,9 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="595"/>
-      <c r="C3" s="597"/>
-      <c r="D3" s="597"/>
+      <c r="B3" s="606"/>
+      <c r="C3" s="608"/>
+      <c r="D3" s="608"/>
       <c r="E3" s="414" t="s">
         <v>320</v>
       </c>
@@ -15322,7 +15409,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="598" t="s">
+      <c r="B4" s="609" t="s">
         <v>323</v>
       </c>
       <c r="C4" s="416" t="s">
@@ -15341,7 +15428,7 @@
       <c r="N4" s="418"/>
     </row>
     <row r="5" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="598"/>
+      <c r="B5" s="609"/>
       <c r="C5" s="416" t="s">
         <v>63</v>
       </c>
@@ -15358,7 +15445,7 @@
       <c r="N5" s="418"/>
     </row>
     <row r="6" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="599"/>
+      <c r="B6" s="610"/>
       <c r="C6" s="419" t="s">
         <v>313</v>
       </c>
@@ -15408,7 +15495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:L5"/>
     </sheetView>
   </sheetViews>
@@ -15419,24 +15506,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="619" t="s">
+      <c r="A1" s="611" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="620"/>
-      <c r="C1" s="600"/>
-      <c r="D1" s="621" t="s">
+      <c r="B1" s="612"/>
+      <c r="C1" s="613"/>
+      <c r="D1" s="614" t="s">
         <v>325</v>
       </c>
-      <c r="E1" s="621"/>
-      <c r="F1" s="601"/>
+      <c r="E1" s="614"/>
+      <c r="F1" s="615"/>
       <c r="G1" s="429" t="s">
         <v>326</v>
       </c>
-      <c r="H1" s="622"/>
-      <c r="I1" s="622"/>
-      <c r="J1" s="622"/>
+      <c r="H1" s="501"/>
+      <c r="I1" s="501"/>
+      <c r="J1" s="501"/>
       <c r="K1" s="430"/>
-      <c r="L1" s="602" t="s">
+      <c r="L1" s="616" t="s">
         <v>327</v>
       </c>
     </row>
@@ -15474,7 +15561,7 @@
       <c r="K2" s="439" t="s">
         <v>331</v>
       </c>
-      <c r="L2" s="603"/>
+      <c r="L2" s="617"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="440"/>
@@ -15482,47 +15569,47 @@
       <c r="C3" s="442" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="604" t="s">
+      <c r="D3" s="618" t="s">
         <v>332</v>
       </c>
-      <c r="E3" s="605"/>
-      <c r="F3" s="606"/>
-      <c r="G3" s="607" t="s">
+      <c r="E3" s="619"/>
+      <c r="F3" s="620"/>
+      <c r="G3" s="621" t="s">
         <v>332</v>
       </c>
-      <c r="H3" s="608"/>
-      <c r="I3" s="608"/>
-      <c r="J3" s="608"/>
-      <c r="K3" s="609"/>
-      <c r="L3" s="603"/>
+      <c r="H3" s="622"/>
+      <c r="I3" s="622"/>
+      <c r="J3" s="622"/>
+      <c r="K3" s="623"/>
+      <c r="L3" s="617"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="623"/>
-      <c r="B4" s="624"/>
-      <c r="C4" s="625"/>
-      <c r="D4" s="626"/>
-      <c r="E4" s="624"/>
-      <c r="F4" s="624"/>
-      <c r="G4" s="624"/>
-      <c r="H4" s="624"/>
-      <c r="I4" s="624"/>
-      <c r="J4" s="624"/>
-      <c r="K4" s="624"/>
-      <c r="L4" s="627"/>
+      <c r="A4" s="502"/>
+      <c r="B4" s="503"/>
+      <c r="C4" s="504"/>
+      <c r="D4" s="505"/>
+      <c r="E4" s="503"/>
+      <c r="F4" s="503"/>
+      <c r="G4" s="503"/>
+      <c r="H4" s="503"/>
+      <c r="I4" s="503"/>
+      <c r="J4" s="503"/>
+      <c r="K4" s="503"/>
+      <c r="L4" s="506"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="628"/>
-      <c r="B5" s="629"/>
-      <c r="C5" s="630"/>
-      <c r="D5" s="631"/>
-      <c r="E5" s="629"/>
-      <c r="F5" s="631"/>
-      <c r="G5" s="629"/>
-      <c r="H5" s="629"/>
-      <c r="I5" s="629"/>
-      <c r="J5" s="629"/>
-      <c r="K5" s="629"/>
-      <c r="L5" s="632"/>
+      <c r="A5" s="507"/>
+      <c r="B5" s="508"/>
+      <c r="C5" s="509"/>
+      <c r="D5" s="510"/>
+      <c r="E5" s="508"/>
+      <c r="F5" s="510"/>
+      <c r="G5" s="508"/>
+      <c r="H5" s="508"/>
+      <c r="I5" s="508"/>
+      <c r="J5" s="508"/>
+      <c r="K5" s="508"/>
+      <c r="L5" s="511"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -15547,23 +15634,23 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="534" t="s">
+      <c r="A1" s="516" t="s">
         <v>333</v>
       </c>
-      <c r="B1" s="535"/>
-      <c r="C1" s="535"/>
-      <c r="D1" s="535"/>
+      <c r="B1" s="517"/>
+      <c r="C1" s="517"/>
+      <c r="D1" s="517"/>
       <c r="E1" s="443"/>
-      <c r="F1" s="615" t="s">
+      <c r="F1" s="629" t="s">
         <v>155</v>
       </c>
-      <c r="G1" s="616"/>
-      <c r="H1" s="616"/>
+      <c r="G1" s="630"/>
+      <c r="H1" s="630"/>
       <c r="I1" s="444"/>
       <c r="J1" s="445"/>
       <c r="K1" s="444"/>
       <c r="L1" s="446"/>
-      <c r="M1" s="610" t="s">
+      <c r="M1" s="624" t="s">
         <v>334</v>
       </c>
       <c r="N1" s="447"/>
@@ -15575,19 +15662,19 @@
       <c r="R1" s="445"/>
       <c r="S1" s="444"/>
       <c r="T1" s="446"/>
-      <c r="U1" s="610" t="s">
+      <c r="U1" s="624" t="s">
         <v>336</v>
       </c>
       <c r="V1" s="447"/>
-      <c r="W1" s="617" t="s">
+      <c r="W1" s="631" t="s">
         <v>337</v>
       </c>
-      <c r="X1" s="617"/>
-      <c r="Y1" s="617"/>
-      <c r="Z1" s="617"/>
-      <c r="AA1" s="617"/>
-      <c r="AB1" s="618"/>
-      <c r="AC1" s="610" t="s">
+      <c r="X1" s="631"/>
+      <c r="Y1" s="631"/>
+      <c r="Z1" s="631"/>
+      <c r="AA1" s="631"/>
+      <c r="AB1" s="632"/>
+      <c r="AC1" s="624" t="s">
         <v>338</v>
       </c>
     </row>
@@ -15601,52 +15688,52 @@
       <c r="C2" s="449" t="s">
         <v>340</v>
       </c>
-      <c r="D2" s="612" t="s">
+      <c r="D2" s="626" t="s">
         <v>341</v>
       </c>
-      <c r="E2" s="612"/>
+      <c r="E2" s="626"/>
       <c r="F2" s="450"/>
-      <c r="G2" s="613" t="s">
+      <c r="G2" s="627" t="s">
         <v>177</v>
       </c>
-      <c r="H2" s="613"/>
-      <c r="I2" s="613" t="s">
+      <c r="H2" s="627"/>
+      <c r="I2" s="627" t="s">
         <v>178</v>
       </c>
-      <c r="J2" s="613"/>
-      <c r="K2" s="613" t="s">
+      <c r="J2" s="627"/>
+      <c r="K2" s="627" t="s">
         <v>179</v>
       </c>
-      <c r="L2" s="614"/>
-      <c r="M2" s="611"/>
+      <c r="L2" s="628"/>
+      <c r="M2" s="625"/>
       <c r="N2" s="451"/>
-      <c r="O2" s="613" t="s">
+      <c r="O2" s="627" t="s">
         <v>177</v>
       </c>
-      <c r="P2" s="613"/>
-      <c r="Q2" s="613" t="s">
+      <c r="P2" s="627"/>
+      <c r="Q2" s="627" t="s">
         <v>178</v>
       </c>
-      <c r="R2" s="613"/>
-      <c r="S2" s="613" t="s">
+      <c r="R2" s="627"/>
+      <c r="S2" s="627" t="s">
         <v>179</v>
       </c>
-      <c r="T2" s="614"/>
-      <c r="U2" s="611"/>
+      <c r="T2" s="628"/>
+      <c r="U2" s="625"/>
       <c r="V2" s="451"/>
-      <c r="W2" s="613" t="s">
+      <c r="W2" s="627" t="s">
         <v>177</v>
       </c>
-      <c r="X2" s="613"/>
-      <c r="Y2" s="613" t="s">
+      <c r="X2" s="627"/>
+      <c r="Y2" s="627" t="s">
         <v>178</v>
       </c>
-      <c r="Z2" s="613"/>
-      <c r="AA2" s="613" t="s">
+      <c r="Z2" s="627"/>
+      <c r="AA2" s="627" t="s">
         <v>179</v>
       </c>
-      <c r="AB2" s="614"/>
-      <c r="AC2" s="611"/>
+      <c r="AB2" s="628"/>
+      <c r="AC2" s="625"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">

</xml_diff>